<commit_message>
changes to the 'salud' statechart
</commit_message>
<xml_diff>
--- a/COVID Contagio Argentina Monte Carlo/Input/Input_Simulador.xlsx
+++ b/COVID Contagio Argentina Monte Carlo/Input/Input_Simulador.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina Monte Carlo\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1E57A7-03ED-453A-93FF-1CB2266A6875}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ED64CA-BD45-4B52-9EBD-06FDB0CE3F41}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="2" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
@@ -4929,7 +4929,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5015,7 +5015,7 @@
         <v>1000</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="63">
         <v>31049</v>
@@ -5056,7 +5056,7 @@
         <v>1000</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="63">
         <v>53940</v>
@@ -5413,7 +5413,7 @@
         <v>10</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="63">
         <v>3176</v>

</xml_diff>

<commit_message>
added trips from abroad containing foreign cases of infection
</commit_message>
<xml_diff>
--- a/COVID Contagio Argentina Monte Carlo/Input/Input_Simulador.xlsx
+++ b/COVID Contagio Argentina Monte Carlo/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina Monte Carlo\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB706D7-DD05-40E6-8BDD-324E66C534A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D301003-30A5-4F23-871A-BB6321F34890}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28830" windowHeight="15750" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="5" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="28" r:id="rId1"/>
@@ -18,17 +18,18 @@
     <sheet name="Perfil Etário" sheetId="2" r:id="rId3"/>
     <sheet name="Probabilidad de Movimiento" sheetId="25" r:id="rId4"/>
     <sheet name="Matriz Origen-Destino" sheetId="3" r:id="rId5"/>
-    <sheet name="Tipos de Movimiento" sheetId="14" r:id="rId6"/>
-    <sheet name="Capacidad Sanitaria" sheetId="30" r:id="rId7"/>
-    <sheet name="Estado Inicial" sheetId="31" r:id="rId8"/>
-    <sheet name="Enfermedad" sheetId="4" r:id="rId9"/>
-    <sheet name="ProbabilidadadecontraerVirus" sheetId="11" r:id="rId10"/>
-    <sheet name="Efecto Severidad en Letalidad" sheetId="16" r:id="rId11"/>
-    <sheet name="Tasa de Letalidad Moderada" sheetId="17" r:id="rId12"/>
-    <sheet name="Tasa de Letalidad Grave" sheetId="18" r:id="rId13"/>
-    <sheet name="Agravamiento" sheetId="19" r:id="rId14"/>
-    <sheet name="Tasa de Enfermedad Moderada" sheetId="20" r:id="rId15"/>
-    <sheet name="Tasa de Enfermedad Grave" sheetId="21" r:id="rId16"/>
+    <sheet name="Movimientos del Exterior" sheetId="32" r:id="rId6"/>
+    <sheet name="Tipos de Movimiento" sheetId="14" r:id="rId7"/>
+    <sheet name="Capacidad Sanitaria" sheetId="30" r:id="rId8"/>
+    <sheet name="Estado Inicial" sheetId="31" r:id="rId9"/>
+    <sheet name="Enfermedad" sheetId="4" r:id="rId10"/>
+    <sheet name="ProbabilidadadecontraerVirus" sheetId="11" r:id="rId11"/>
+    <sheet name="Efecto Severidad en Letalidad" sheetId="16" r:id="rId12"/>
+    <sheet name="Tasa de Letalidad Moderada" sheetId="17" r:id="rId13"/>
+    <sheet name="Tasa de Letalidad Grave" sheetId="18" r:id="rId14"/>
+    <sheet name="Agravamiento" sheetId="19" r:id="rId15"/>
+    <sheet name="Tasa de Enfermedad Moderada" sheetId="20" r:id="rId16"/>
+    <sheet name="Tasa de Enfermedad Grave" sheetId="21" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Perfil Etário'!$A$1:$F$2725</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="220">
   <si>
     <t>Santa Fe</t>
   </si>
@@ -1210,87 +1211,6 @@
   </si>
   <si>
     <r>
-      <t>Para estimar el valor de la cantidad de</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Camas de Aislamiento</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> se contabilizaron las suigientes camas disponibles en hospitales: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t>Uso General, Hopital Dia ??? , Usos Especiales, Internación Prolongadas y No Discriminadas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t>No se han tenido</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> en cuenta las camas reservadas para</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Maternindad, Neonatología o Pediatricas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Graphik"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>La hoja de Capacidad Sanitaria contiene la información correspondiente a la</t>
     </r>
     <r>
@@ -1575,17 +1495,117 @@
   <si>
     <t>2. Probabilidad de Ocurrencia [%]</t>
   </si>
+  <si>
+    <r>
+      <t>Para estimar el valor de la cantidad de</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Camas de Aislamiento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> se contabilizaron las suigientes camas disponibles en hospitales: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t>Uso General, Uso Común , Usos Especiales, Internación Prolongadas y No Discriminadas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t>No se han tenido</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> en cuenta las camas reservadas para</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Maternindad, Neonatología o Pediatricas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Graphik"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Id Región Destino</t>
+  </si>
+  <si>
+    <t>2. Nombre Región Destino</t>
+  </si>
+  <si>
+    <t>3. Probabilidad</t>
+  </si>
+  <si>
+    <t>4. Probabilidad Acumulada</t>
+  </si>
+  <si>
+    <t>Cantidad de Ingresos por Día [personas]</t>
+  </si>
+  <si>
+    <t>Probabilidad de Ingreso Infectado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m\-d"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="173" formatCode="0.000"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -2000,7 +2020,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2206,32 +2226,24 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2242,32 +2254,53 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2758,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFB5D56-B68E-4E9D-9EC4-1DBA7AFCA152}">
   <dimension ref="A1:AS83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q91" sqref="Q91"/>
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2805,139 +2838,139 @@
     </row>
     <row r="3" spans="2:45" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:45" ht="15" customHeight="1">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="96"/>
     </row>
     <row r="5" spans="2:45" ht="22.5" customHeight="1">
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="Q5" s="104" t="s">
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="Q5" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="104"/>
-      <c r="V5" s="104"/>
-      <c r="W5" s="104"/>
-      <c r="X5" s="104"/>
-      <c r="Y5" s="104"/>
-      <c r="Z5" s="104"/>
-      <c r="AA5" s="104"/>
-      <c r="AB5" s="104"/>
-      <c r="AC5" s="104"/>
-      <c r="AD5" s="104"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="102"/>
+      <c r="V5" s="102"/>
+      <c r="W5" s="102"/>
+      <c r="X5" s="102"/>
+      <c r="Y5" s="102"/>
+      <c r="Z5" s="102"/>
+      <c r="AA5" s="102"/>
+      <c r="AB5" s="102"/>
+      <c r="AC5" s="102"/>
+      <c r="AD5" s="102"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
     </row>
     <row r="6" spans="2:45">
-      <c r="Q6" s="105" t="s">
+      <c r="Q6" s="101" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="105"/>
-      <c r="S6" s="105"/>
-      <c r="T6" s="105"/>
-      <c r="U6" s="105"/>
-      <c r="V6" s="105"/>
-      <c r="W6" s="105"/>
-      <c r="X6" s="105"/>
-      <c r="Y6" s="105"/>
-      <c r="Z6" s="105"/>
-      <c r="AA6" s="105"/>
-      <c r="AB6" s="105"/>
-      <c r="AC6" s="105"/>
-      <c r="AD6" s="105"/>
+      <c r="R6" s="101"/>
+      <c r="S6" s="101"/>
+      <c r="T6" s="101"/>
+      <c r="U6" s="101"/>
+      <c r="V6" s="101"/>
+      <c r="W6" s="101"/>
+      <c r="X6" s="101"/>
+      <c r="Y6" s="101"/>
+      <c r="Z6" s="101"/>
+      <c r="AA6" s="101"/>
+      <c r="AB6" s="101"/>
+      <c r="AC6" s="101"/>
+      <c r="AD6" s="101"/>
     </row>
     <row r="7" spans="2:45">
-      <c r="Q7" s="105"/>
-      <c r="R7" s="105"/>
-      <c r="S7" s="105"/>
-      <c r="T7" s="105"/>
-      <c r="U7" s="105"/>
-      <c r="V7" s="105"/>
-      <c r="W7" s="105"/>
-      <c r="X7" s="105"/>
-      <c r="Y7" s="105"/>
-      <c r="Z7" s="105"/>
-      <c r="AA7" s="105"/>
-      <c r="AB7" s="105"/>
-      <c r="AC7" s="105"/>
-      <c r="AD7" s="105"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
+      <c r="S7" s="101"/>
+      <c r="T7" s="101"/>
+      <c r="U7" s="101"/>
+      <c r="V7" s="101"/>
+      <c r="W7" s="101"/>
+      <c r="X7" s="101"/>
+      <c r="Y7" s="101"/>
+      <c r="Z7" s="101"/>
+      <c r="AA7" s="101"/>
+      <c r="AB7" s="101"/>
+      <c r="AC7" s="101"/>
+      <c r="AD7" s="101"/>
     </row>
     <row r="8" spans="2:45" ht="15" customHeight="1">
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="89"/>
-      <c r="L8" s="89"/>
-      <c r="M8" s="89"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="Q8" s="105"/>
-      <c r="R8" s="105"/>
-      <c r="S8" s="105"/>
-      <c r="T8" s="105"/>
-      <c r="U8" s="105"/>
-      <c r="V8" s="105"/>
-      <c r="W8" s="105"/>
-      <c r="X8" s="105"/>
-      <c r="Y8" s="105"/>
-      <c r="Z8" s="105"/>
-      <c r="AA8" s="105"/>
-      <c r="AB8" s="105"/>
-      <c r="AC8" s="105"/>
-      <c r="AD8" s="105"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="96"/>
+      <c r="O8" s="96"/>
+      <c r="Q8" s="101"/>
+      <c r="R8" s="101"/>
+      <c r="S8" s="101"/>
+      <c r="T8" s="101"/>
+      <c r="U8" s="101"/>
+      <c r="V8" s="101"/>
+      <c r="W8" s="101"/>
+      <c r="X8" s="101"/>
+      <c r="Y8" s="101"/>
+      <c r="Z8" s="101"/>
+      <c r="AA8" s="101"/>
+      <c r="AB8" s="101"/>
+      <c r="AC8" s="101"/>
+      <c r="AD8" s="101"/>
     </row>
     <row r="9" spans="2:45" ht="17.25" customHeight="1">
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="89"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="96"/>
     </row>
     <row r="12" spans="2:45" ht="17.25" customHeight="1">
       <c r="D12" s="15" t="s">
@@ -3012,41 +3045,41 @@
       <c r="M19" s="99"/>
     </row>
     <row r="22" spans="2:43">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="104"/>
+      <c r="O22" s="104"/>
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1"/>
     <row r="24" spans="2:43" ht="17.25">
-      <c r="B24" s="90" t="s">
+      <c r="B24" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
-      <c r="J24" s="90"/>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="90"/>
-      <c r="O24" s="90"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="103"/>
+      <c r="J24" s="103"/>
+      <c r="K24" s="103"/>
+      <c r="L24" s="103"/>
+      <c r="M24" s="103"/>
+      <c r="N24" s="103"/>
+      <c r="O24" s="103"/>
     </row>
     <row r="25" spans="2:43">
       <c r="R25" s="23"/>
@@ -3067,37 +3100,37 @@
         <v>96</v>
       </c>
       <c r="R26" s="26"/>
-      <c r="S26" s="102" t="s">
+      <c r="S26" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="T26" s="102"/>
-      <c r="U26" s="102"/>
-      <c r="V26" s="102"/>
-      <c r="W26" s="102"/>
-      <c r="X26" s="102"/>
-      <c r="Y26" s="102"/>
-      <c r="Z26" s="102"/>
-      <c r="AA26" s="102"/>
-      <c r="AB26" s="102"/>
+      <c r="T26" s="108"/>
+      <c r="U26" s="108"/>
+      <c r="V26" s="108"/>
+      <c r="W26" s="108"/>
+      <c r="X26" s="108"/>
+      <c r="Y26" s="108"/>
+      <c r="Z26" s="108"/>
+      <c r="AA26" s="108"/>
+      <c r="AB26" s="108"/>
       <c r="AC26" s="27"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1">
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="89"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="89"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="89"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="96"/>
+      <c r="J27" s="96"/>
+      <c r="K27" s="96"/>
+      <c r="L27" s="96"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="96"/>
+      <c r="O27" s="96"/>
       <c r="R27" s="26"/>
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
@@ -3122,51 +3155,51 @@
       <c r="AQ27" s="18"/>
     </row>
     <row r="28" spans="2:43" ht="15" customHeight="1">
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="89"/>
-      <c r="N28" s="89"/>
-      <c r="O28" s="89"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="96"/>
+      <c r="O28" s="96"/>
       <c r="R28" s="26"/>
       <c r="AC28" s="27"/>
     </row>
     <row r="29" spans="2:43" ht="17.25">
-      <c r="B29" s="89"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="89"/>
-      <c r="M29" s="89"/>
-      <c r="N29" s="89"/>
-      <c r="O29" s="89"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="96"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="96"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="96"/>
+      <c r="O29" s="96"/>
       <c r="R29" s="26"/>
-      <c r="S29" s="101" t="s">
+      <c r="S29" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="101"/>
-      <c r="U29" s="101"/>
-      <c r="V29" s="101"/>
-      <c r="W29" s="101"/>
-      <c r="X29" s="101"/>
-      <c r="Y29" s="101"/>
-      <c r="Z29" s="101"/>
-      <c r="AA29" s="101"/>
-      <c r="AB29" s="101"/>
+      <c r="T29" s="107"/>
+      <c r="U29" s="107"/>
+      <c r="V29" s="107"/>
+      <c r="W29" s="107"/>
+      <c r="X29" s="107"/>
+      <c r="Y29" s="107"/>
+      <c r="Z29" s="107"/>
+      <c r="AA29" s="107"/>
+      <c r="AB29" s="107"/>
       <c r="AC29" s="27"/>
     </row>
     <row r="30" spans="2:43">
@@ -3184,52 +3217,52 @@
       <c r="AC30" s="27"/>
     </row>
     <row r="31" spans="2:43" ht="17.25">
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="96" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="89"/>
-      <c r="D31" s="89"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="89"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="89"/>
-      <c r="I31" s="89"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="89"/>
-      <c r="L31" s="89"/>
-      <c r="M31" s="89"/>
-      <c r="N31" s="89"/>
-      <c r="O31" s="89"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="96"/>
+      <c r="H31" s="96"/>
+      <c r="I31" s="96"/>
+      <c r="J31" s="96"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="96"/>
+      <c r="M31" s="96"/>
+      <c r="N31" s="96"/>
+      <c r="O31" s="96"/>
       <c r="R31" s="26"/>
       <c r="S31" s="18"/>
       <c r="T31" s="18"/>
       <c r="U31" s="18"/>
-      <c r="V31" s="97" t="s">
+      <c r="V31" s="105" t="s">
         <v>109</v>
       </c>
-      <c r="W31" s="97"/>
-      <c r="X31" s="97"/>
-      <c r="Y31" s="97"/>
-      <c r="Z31" s="97"/>
+      <c r="W31" s="105"/>
+      <c r="X31" s="105"/>
+      <c r="Y31" s="105"/>
+      <c r="Z31" s="105"/>
       <c r="AA31" s="18"/>
       <c r="AB31" s="18"/>
       <c r="AC31" s="27"/>
     </row>
     <row r="32" spans="2:43" ht="15" customHeight="1">
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="89"/>
-      <c r="I32" s="89"/>
-      <c r="J32" s="89"/>
-      <c r="K32" s="89"/>
-      <c r="L32" s="89"/>
-      <c r="M32" s="89"/>
-      <c r="N32" s="89"/>
-      <c r="O32" s="89"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="96"/>
+      <c r="I32" s="96"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="96"/>
+      <c r="L32" s="96"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="96"/>
+      <c r="O32" s="96"/>
       <c r="R32" s="26"/>
       <c r="S32" s="18"/>
       <c r="T32" s="18"/>
@@ -3244,61 +3277,61 @@
       <c r="AC32" s="27"/>
     </row>
     <row r="33" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B33" s="89" t="s">
+      <c r="B33" s="96" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="89"/>
-      <c r="I33" s="89"/>
-      <c r="J33" s="89"/>
-      <c r="K33" s="89"/>
-      <c r="L33" s="89"/>
-      <c r="M33" s="89"/>
-      <c r="N33" s="89"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="96"/>
+      <c r="G33" s="96"/>
+      <c r="H33" s="96"/>
+      <c r="I33" s="96"/>
+      <c r="J33" s="96"/>
+      <c r="K33" s="96"/>
+      <c r="L33" s="96"/>
+      <c r="M33" s="96"/>
+      <c r="N33" s="96"/>
       <c r="R33" s="26"/>
-      <c r="S33" s="93" t="s">
+      <c r="S33" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="93"/>
-      <c r="U33" s="93"/>
-      <c r="V33" s="93"/>
-      <c r="W33" s="93"/>
-      <c r="X33" s="93"/>
-      <c r="Y33" s="93"/>
-      <c r="Z33" s="93"/>
-      <c r="AA33" s="93"/>
-      <c r="AB33" s="93"/>
+      <c r="T33" s="109"/>
+      <c r="U33" s="109"/>
+      <c r="V33" s="109"/>
+      <c r="W33" s="109"/>
+      <c r="X33" s="109"/>
+      <c r="Y33" s="109"/>
+      <c r="Z33" s="109"/>
+      <c r="AA33" s="109"/>
+      <c r="AB33" s="109"/>
       <c r="AC33" s="27"/>
     </row>
     <row r="34" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B34" s="89"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="89"/>
-      <c r="H34" s="89"/>
-      <c r="I34" s="89"/>
-      <c r="J34" s="89"/>
-      <c r="K34" s="89"/>
-      <c r="L34" s="89"/>
-      <c r="M34" s="89"/>
-      <c r="N34" s="89"/>
+      <c r="B34" s="96"/>
+      <c r="C34" s="96"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="96"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="96"/>
+      <c r="L34" s="96"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="96"/>
       <c r="R34" s="26"/>
-      <c r="S34" s="93"/>
-      <c r="T34" s="93"/>
-      <c r="U34" s="93"/>
-      <c r="V34" s="93"/>
-      <c r="W34" s="93"/>
-      <c r="X34" s="93"/>
-      <c r="Y34" s="93"/>
-      <c r="Z34" s="93"/>
-      <c r="AA34" s="93"/>
-      <c r="AB34" s="93"/>
+      <c r="S34" s="109"/>
+      <c r="T34" s="109"/>
+      <c r="U34" s="109"/>
+      <c r="V34" s="109"/>
+      <c r="W34" s="109"/>
+      <c r="X34" s="109"/>
+      <c r="Y34" s="109"/>
+      <c r="Z34" s="109"/>
+      <c r="AA34" s="109"/>
+      <c r="AB34" s="109"/>
       <c r="AC34" s="27"/>
     </row>
     <row r="35" spans="2:32">
@@ -3336,67 +3369,67 @@
     </row>
     <row r="37" spans="2:32">
       <c r="R37" s="26"/>
-      <c r="S37" s="106" t="s">
+      <c r="S37" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="T37" s="106"/>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="106"/>
-      <c r="X37" s="106"/>
-      <c r="Y37" s="106"/>
-      <c r="Z37" s="106"/>
-      <c r="AA37" s="106"/>
-      <c r="AB37" s="106"/>
+      <c r="T37" s="110"/>
+      <c r="U37" s="110"/>
+      <c r="V37" s="110"/>
+      <c r="W37" s="110"/>
+      <c r="X37" s="110"/>
+      <c r="Y37" s="110"/>
+      <c r="Z37" s="110"/>
+      <c r="AA37" s="110"/>
+      <c r="AB37" s="110"/>
       <c r="AC37" s="27"/>
       <c r="AF37" s="9"/>
     </row>
     <row r="38" spans="2:32">
-      <c r="B38" s="89" t="s">
+      <c r="B38" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="89"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="89"/>
-      <c r="L38" s="89"/>
-      <c r="M38" s="89"/>
-      <c r="N38" s="89"/>
-      <c r="O38" s="89"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
+      <c r="G38" s="96"/>
+      <c r="H38" s="96"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="96"/>
+      <c r="K38" s="96"/>
+      <c r="L38" s="96"/>
+      <c r="M38" s="96"/>
+      <c r="N38" s="96"/>
+      <c r="O38" s="96"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="106"/>
-      <c r="T38" s="106"/>
-      <c r="U38" s="106"/>
-      <c r="V38" s="106"/>
-      <c r="W38" s="106"/>
-      <c r="X38" s="106"/>
-      <c r="Y38" s="106"/>
-      <c r="Z38" s="106"/>
-      <c r="AA38" s="106"/>
-      <c r="AB38" s="106"/>
+      <c r="S38" s="110"/>
+      <c r="T38" s="110"/>
+      <c r="U38" s="110"/>
+      <c r="V38" s="110"/>
+      <c r="W38" s="110"/>
+      <c r="X38" s="110"/>
+      <c r="Y38" s="110"/>
+      <c r="Z38" s="110"/>
+      <c r="AA38" s="110"/>
+      <c r="AB38" s="110"/>
       <c r="AC38" s="27"/>
       <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="2:32">
-      <c r="B39" s="89"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="89"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="89"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="89"/>
-      <c r="M39" s="89"/>
-      <c r="N39" s="89"/>
-      <c r="O39" s="89"/>
+      <c r="B39" s="96"/>
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="96"/>
+      <c r="J39" s="96"/>
+      <c r="K39" s="96"/>
+      <c r="L39" s="96"/>
+      <c r="M39" s="96"/>
+      <c r="N39" s="96"/>
+      <c r="O39" s="96"/>
       <c r="R39" s="26"/>
       <c r="S39" s="18"/>
       <c r="T39" s="19"/>
@@ -3416,34 +3449,34 @@
       <c r="S40" s="18"/>
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
-      <c r="V40" s="103" t="s">
+      <c r="V40" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="W40" s="103"/>
-      <c r="X40" s="103"/>
-      <c r="Y40" s="103"/>
-      <c r="Z40" s="103"/>
+      <c r="W40" s="106"/>
+      <c r="X40" s="106"/>
+      <c r="Y40" s="106"/>
+      <c r="Z40" s="106"/>
       <c r="AA40" s="19"/>
       <c r="AB40" s="19"/>
       <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="2:32" ht="17.25">
-      <c r="B41" s="90" t="s">
+      <c r="B41" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="90"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="90"/>
-      <c r="N41" s="90"/>
-      <c r="O41" s="90"/>
+      <c r="C41" s="103"/>
+      <c r="D41" s="103"/>
+      <c r="E41" s="103"/>
+      <c r="F41" s="103"/>
+      <c r="G41" s="103"/>
+      <c r="H41" s="103"/>
+      <c r="I41" s="103"/>
+      <c r="J41" s="103"/>
+      <c r="K41" s="103"/>
+      <c r="L41" s="103"/>
+      <c r="M41" s="103"/>
+      <c r="N41" s="103"/>
+      <c r="O41" s="103"/>
       <c r="R41" s="26"/>
       <c r="S41" s="18"/>
       <c r="T41" s="18"/>
@@ -3459,18 +3492,18 @@
     </row>
     <row r="42" spans="2:32" ht="17.25">
       <c r="R42" s="26"/>
-      <c r="S42" s="101" t="s">
+      <c r="S42" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="T42" s="101"/>
-      <c r="U42" s="101"/>
-      <c r="V42" s="101"/>
-      <c r="W42" s="101"/>
-      <c r="X42" s="101"/>
-      <c r="Y42" s="101"/>
-      <c r="Z42" s="101"/>
-      <c r="AA42" s="101"/>
-      <c r="AB42" s="101"/>
+      <c r="T42" s="107"/>
+      <c r="U42" s="107"/>
+      <c r="V42" s="107"/>
+      <c r="W42" s="107"/>
+      <c r="X42" s="107"/>
+      <c r="Y42" s="107"/>
+      <c r="Z42" s="107"/>
+      <c r="AA42" s="107"/>
+      <c r="AB42" s="107"/>
       <c r="AC42" s="27"/>
     </row>
     <row r="43" spans="2:32" ht="17.25">
@@ -3505,63 +3538,63 @@
       <c r="AC44" s="27"/>
     </row>
     <row r="45" spans="2:32">
-      <c r="B45" s="89" t="s">
+      <c r="B45" s="96" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="89"/>
-      <c r="G45" s="89"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
-      <c r="L45" s="89"/>
-      <c r="M45" s="89"/>
-      <c r="N45" s="89"/>
-      <c r="O45" s="89"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="96"/>
+      <c r="G45" s="96"/>
+      <c r="H45" s="96"/>
+      <c r="I45" s="96"/>
+      <c r="J45" s="96"/>
+      <c r="K45" s="96"/>
+      <c r="L45" s="96"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="96"/>
+      <c r="O45" s="96"/>
       <c r="R45" s="26"/>
-      <c r="S45" s="93" t="s">
+      <c r="S45" s="109" t="s">
         <v>113</v>
       </c>
-      <c r="T45" s="93"/>
-      <c r="U45" s="93"/>
-      <c r="V45" s="93"/>
-      <c r="W45" s="93"/>
-      <c r="X45" s="93"/>
-      <c r="Y45" s="93"/>
-      <c r="Z45" s="93"/>
-      <c r="AA45" s="93"/>
-      <c r="AB45" s="93"/>
+      <c r="T45" s="109"/>
+      <c r="U45" s="109"/>
+      <c r="V45" s="109"/>
+      <c r="W45" s="109"/>
+      <c r="X45" s="109"/>
+      <c r="Y45" s="109"/>
+      <c r="Z45" s="109"/>
+      <c r="AA45" s="109"/>
+      <c r="AB45" s="109"/>
       <c r="AC45" s="27"/>
     </row>
     <row r="46" spans="2:32" ht="15" customHeight="1">
-      <c r="B46" s="89"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="89"/>
-      <c r="G46" s="89"/>
-      <c r="H46" s="89"/>
-      <c r="I46" s="89"/>
-      <c r="J46" s="89"/>
-      <c r="K46" s="89"/>
-      <c r="L46" s="89"/>
-      <c r="M46" s="89"/>
-      <c r="N46" s="89"/>
-      <c r="O46" s="89"/>
+      <c r="B46" s="96"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
+      <c r="H46" s="96"/>
+      <c r="I46" s="96"/>
+      <c r="J46" s="96"/>
+      <c r="K46" s="96"/>
+      <c r="L46" s="96"/>
+      <c r="M46" s="96"/>
+      <c r="N46" s="96"/>
+      <c r="O46" s="96"/>
       <c r="R46" s="26"/>
-      <c r="S46" s="93"/>
-      <c r="T46" s="93"/>
-      <c r="U46" s="93"/>
-      <c r="V46" s="93"/>
-      <c r="W46" s="93"/>
-      <c r="X46" s="93"/>
-      <c r="Y46" s="93"/>
-      <c r="Z46" s="93"/>
-      <c r="AA46" s="93"/>
-      <c r="AB46" s="93"/>
+      <c r="S46" s="109"/>
+      <c r="T46" s="109"/>
+      <c r="U46" s="109"/>
+      <c r="V46" s="109"/>
+      <c r="W46" s="109"/>
+      <c r="X46" s="109"/>
+      <c r="Y46" s="109"/>
+      <c r="Z46" s="109"/>
+      <c r="AA46" s="109"/>
+      <c r="AB46" s="109"/>
       <c r="AC46" s="27"/>
     </row>
     <row r="47" spans="2:32" ht="15" customHeight="1">
@@ -3586,13 +3619,13 @@
       <c r="S48" s="18"/>
       <c r="T48" s="18"/>
       <c r="U48" s="18"/>
-      <c r="V48" s="94" t="s">
+      <c r="V48" s="112" t="s">
         <v>114</v>
       </c>
-      <c r="W48" s="94"/>
-      <c r="X48" s="94"/>
-      <c r="Y48" s="94"/>
-      <c r="Z48" s="94"/>
+      <c r="W48" s="112"/>
+      <c r="X48" s="112"/>
+      <c r="Y48" s="112"/>
+      <c r="Z48" s="112"/>
       <c r="AA48" s="18"/>
       <c r="AB48" s="18"/>
       <c r="AC48" s="27"/>
@@ -3612,22 +3645,22 @@
       <c r="AC49" s="27"/>
     </row>
     <row r="50" spans="2:43">
-      <c r="B50" s="89" t="s">
+      <c r="B50" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
-      <c r="G50" s="89"/>
-      <c r="H50" s="89"/>
-      <c r="I50" s="89"/>
-      <c r="J50" s="89"/>
-      <c r="K50" s="89"/>
-      <c r="L50" s="89"/>
-      <c r="M50" s="89"/>
-      <c r="N50" s="89"/>
-      <c r="O50" s="89"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="96"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96"/>
+      <c r="G50" s="96"/>
+      <c r="H50" s="96"/>
+      <c r="I50" s="96"/>
+      <c r="J50" s="96"/>
+      <c r="K50" s="96"/>
+      <c r="L50" s="96"/>
+      <c r="M50" s="96"/>
+      <c r="N50" s="96"/>
+      <c r="O50" s="96"/>
       <c r="R50" s="26"/>
       <c r="S50" s="95" t="s">
         <v>115</v>
@@ -3644,20 +3677,20 @@
       <c r="AC50" s="27"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1">
-      <c r="B51" s="89"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="89"/>
-      <c r="E51" s="89"/>
-      <c r="F51" s="89"/>
-      <c r="G51" s="89"/>
-      <c r="H51" s="89"/>
-      <c r="I51" s="89"/>
-      <c r="J51" s="89"/>
-      <c r="K51" s="89"/>
-      <c r="L51" s="89"/>
-      <c r="M51" s="89"/>
-      <c r="N51" s="89"/>
-      <c r="O51" s="89"/>
+      <c r="B51" s="96"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="96"/>
+      <c r="E51" s="96"/>
+      <c r="F51" s="96"/>
+      <c r="G51" s="96"/>
+      <c r="H51" s="96"/>
+      <c r="I51" s="96"/>
+      <c r="J51" s="96"/>
+      <c r="K51" s="96"/>
+      <c r="L51" s="96"/>
+      <c r="M51" s="96"/>
+      <c r="N51" s="96"/>
+      <c r="O51" s="96"/>
       <c r="R51" s="26"/>
       <c r="S51" s="18"/>
       <c r="T51" s="18"/>
@@ -3729,22 +3762,22 @@
       <c r="AC54" s="27"/>
     </row>
     <row r="55" spans="2:43">
-      <c r="B55" s="89" t="s">
+      <c r="B55" s="96" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="89"/>
-      <c r="D55" s="89"/>
-      <c r="E55" s="89"/>
-      <c r="F55" s="89"/>
-      <c r="G55" s="89"/>
-      <c r="H55" s="89"/>
-      <c r="I55" s="89"/>
-      <c r="J55" s="89"/>
-      <c r="K55" s="89"/>
-      <c r="L55" s="89"/>
-      <c r="M55" s="89"/>
-      <c r="N55" s="89"/>
-      <c r="O55" s="89"/>
+      <c r="C55" s="96"/>
+      <c r="D55" s="96"/>
+      <c r="E55" s="96"/>
+      <c r="F55" s="96"/>
+      <c r="G55" s="96"/>
+      <c r="H55" s="96"/>
+      <c r="I55" s="96"/>
+      <c r="J55" s="96"/>
+      <c r="K55" s="96"/>
+      <c r="L55" s="96"/>
+      <c r="M55" s="96"/>
+      <c r="N55" s="96"/>
+      <c r="O55" s="96"/>
       <c r="R55" s="28"/>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
@@ -3759,276 +3792,276 @@
       <c r="AC55" s="30"/>
     </row>
     <row r="56" spans="2:43">
-      <c r="B56" s="89"/>
-      <c r="C56" s="89"/>
-      <c r="D56" s="89"/>
-      <c r="E56" s="89"/>
-      <c r="F56" s="89"/>
-      <c r="G56" s="89"/>
-      <c r="H56" s="89"/>
-      <c r="I56" s="89"/>
-      <c r="J56" s="89"/>
-      <c r="K56" s="89"/>
-      <c r="L56" s="89"/>
-      <c r="M56" s="89"/>
-      <c r="N56" s="89"/>
-      <c r="O56" s="89"/>
+      <c r="B56" s="96"/>
+      <c r="C56" s="96"/>
+      <c r="D56" s="96"/>
+      <c r="E56" s="96"/>
+      <c r="F56" s="96"/>
+      <c r="G56" s="96"/>
+      <c r="H56" s="96"/>
+      <c r="I56" s="96"/>
+      <c r="J56" s="96"/>
+      <c r="K56" s="96"/>
+      <c r="L56" s="96"/>
+      <c r="M56" s="96"/>
+      <c r="N56" s="96"/>
+      <c r="O56" s="96"/>
     </row>
     <row r="58" spans="2:43" ht="17.25">
-      <c r="B58" s="90" t="s">
+      <c r="B58" s="103" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="90"/>
-      <c r="D58" s="90"/>
-      <c r="E58" s="90"/>
-      <c r="F58" s="90"/>
-      <c r="G58" s="90"/>
-      <c r="H58" s="90"/>
-      <c r="I58" s="90"/>
-      <c r="J58" s="90"/>
-      <c r="K58" s="90"/>
-      <c r="L58" s="90"/>
-      <c r="M58" s="90"/>
-      <c r="N58" s="90"/>
-      <c r="O58" s="90"/>
-      <c r="Q58" s="91" t="s">
+      <c r="C58" s="103"/>
+      <c r="D58" s="103"/>
+      <c r="E58" s="103"/>
+      <c r="F58" s="103"/>
+      <c r="G58" s="103"/>
+      <c r="H58" s="103"/>
+      <c r="I58" s="103"/>
+      <c r="J58" s="103"/>
+      <c r="K58" s="103"/>
+      <c r="L58" s="103"/>
+      <c r="M58" s="103"/>
+      <c r="N58" s="103"/>
+      <c r="O58" s="103"/>
+      <c r="Q58" s="111" t="s">
         <v>169</v>
       </c>
-      <c r="R58" s="91"/>
-      <c r="S58" s="91"/>
-      <c r="T58" s="91"/>
-      <c r="U58" s="91"/>
-      <c r="V58" s="91"/>
-      <c r="W58" s="91"/>
-      <c r="X58" s="91"/>
-      <c r="Y58" s="91"/>
-      <c r="Z58" s="91"/>
-      <c r="AA58" s="91"/>
-      <c r="AB58" s="91"/>
-      <c r="AC58" s="91"/>
-      <c r="AD58" s="91"/>
+      <c r="R58" s="111"/>
+      <c r="S58" s="111"/>
+      <c r="T58" s="111"/>
+      <c r="U58" s="111"/>
+      <c r="V58" s="111"/>
+      <c r="W58" s="111"/>
+      <c r="X58" s="111"/>
+      <c r="Y58" s="111"/>
+      <c r="Z58" s="111"/>
+      <c r="AA58" s="111"/>
+      <c r="AB58" s="111"/>
+      <c r="AC58" s="111"/>
+      <c r="AD58" s="111"/>
     </row>
     <row r="60" spans="2:43" ht="17.25">
-      <c r="B60" s="92" t="s">
-        <v>199</v>
-      </c>
-      <c r="C60" s="92"/>
-      <c r="D60" s="92"/>
-      <c r="E60" s="92"/>
-      <c r="F60" s="92"/>
-      <c r="G60" s="92"/>
-      <c r="H60" s="92"/>
-      <c r="I60" s="92"/>
-      <c r="J60" s="92"/>
-      <c r="K60" s="92"/>
-      <c r="L60" s="92"/>
-      <c r="M60" s="92"/>
-      <c r="N60" s="92"/>
-      <c r="O60" s="92"/>
+      <c r="B60" s="97" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="97"/>
+      <c r="D60" s="97"/>
+      <c r="E60" s="97"/>
+      <c r="F60" s="97"/>
+      <c r="G60" s="97"/>
+      <c r="H60" s="97"/>
+      <c r="I60" s="97"/>
+      <c r="J60" s="97"/>
+      <c r="K60" s="97"/>
+      <c r="L60" s="97"/>
+      <c r="M60" s="97"/>
+      <c r="N60" s="97"/>
+      <c r="O60" s="97"/>
       <c r="Q60" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="2:43">
-      <c r="B61" s="92"/>
-      <c r="C61" s="92"/>
-      <c r="D61" s="92"/>
-      <c r="E61" s="92"/>
-      <c r="F61" s="92"/>
-      <c r="G61" s="92"/>
-      <c r="H61" s="92"/>
-      <c r="I61" s="92"/>
-      <c r="J61" s="92"/>
-      <c r="K61" s="92"/>
-      <c r="L61" s="92"/>
-      <c r="M61" s="92"/>
-      <c r="N61" s="92"/>
-      <c r="O61" s="92"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="97"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="97"/>
+      <c r="G61" s="97"/>
+      <c r="H61" s="97"/>
+      <c r="I61" s="97"/>
+      <c r="J61" s="97"/>
+      <c r="K61" s="97"/>
+      <c r="L61" s="97"/>
+      <c r="M61" s="97"/>
+      <c r="N61" s="97"/>
+      <c r="O61" s="97"/>
     </row>
     <row r="62" spans="2:43">
-      <c r="Q62" s="89" t="s">
+      <c r="Q62" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="R62" s="89"/>
-      <c r="S62" s="89"/>
-      <c r="T62" s="89"/>
-      <c r="U62" s="89"/>
-      <c r="V62" s="89"/>
-      <c r="W62" s="89"/>
-      <c r="X62" s="89"/>
-      <c r="Y62" s="89"/>
-      <c r="Z62" s="89"/>
-      <c r="AA62" s="89"/>
-      <c r="AB62" s="89"/>
-      <c r="AC62" s="89"/>
-      <c r="AD62" s="89"/>
+      <c r="R62" s="96"/>
+      <c r="S62" s="96"/>
+      <c r="T62" s="96"/>
+      <c r="U62" s="96"/>
+      <c r="V62" s="96"/>
+      <c r="W62" s="96"/>
+      <c r="X62" s="96"/>
+      <c r="Y62" s="96"/>
+      <c r="Z62" s="96"/>
+      <c r="AA62" s="96"/>
+      <c r="AB62" s="96"/>
+      <c r="AC62" s="96"/>
+      <c r="AD62" s="96"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1">
-      <c r="B63" s="92" t="s">
-        <v>198</v>
-      </c>
-      <c r="C63" s="92"/>
-      <c r="D63" s="92"/>
-      <c r="E63" s="92"/>
-      <c r="F63" s="92"/>
-      <c r="G63" s="92"/>
-      <c r="H63" s="92"/>
-      <c r="I63" s="92"/>
-      <c r="J63" s="92"/>
-      <c r="K63" s="92"/>
-      <c r="L63" s="92"/>
-      <c r="M63" s="92"/>
-      <c r="N63" s="92"/>
-      <c r="O63" s="92"/>
-      <c r="Q63" s="89"/>
-      <c r="R63" s="89"/>
-      <c r="S63" s="89"/>
-      <c r="T63" s="89"/>
-      <c r="U63" s="89"/>
-      <c r="V63" s="89"/>
-      <c r="W63" s="89"/>
-      <c r="X63" s="89"/>
-      <c r="Y63" s="89"/>
-      <c r="Z63" s="89"/>
-      <c r="AA63" s="89"/>
-      <c r="AB63" s="89"/>
-      <c r="AC63" s="89"/>
-      <c r="AD63" s="89"/>
+      <c r="B63" s="97" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="97"/>
+      <c r="D63" s="97"/>
+      <c r="E63" s="97"/>
+      <c r="F63" s="97"/>
+      <c r="G63" s="97"/>
+      <c r="H63" s="97"/>
+      <c r="I63" s="97"/>
+      <c r="J63" s="97"/>
+      <c r="K63" s="97"/>
+      <c r="L63" s="97"/>
+      <c r="M63" s="97"/>
+      <c r="N63" s="97"/>
+      <c r="O63" s="97"/>
+      <c r="Q63" s="96"/>
+      <c r="R63" s="96"/>
+      <c r="S63" s="96"/>
+      <c r="T63" s="96"/>
+      <c r="U63" s="96"/>
+      <c r="V63" s="96"/>
+      <c r="W63" s="96"/>
+      <c r="X63" s="96"/>
+      <c r="Y63" s="96"/>
+      <c r="Z63" s="96"/>
+      <c r="AA63" s="96"/>
+      <c r="AB63" s="96"/>
+      <c r="AC63" s="96"/>
+      <c r="AD63" s="96"/>
     </row>
     <row r="64" spans="2:43">
-      <c r="B64" s="92"/>
-      <c r="C64" s="92"/>
-      <c r="D64" s="92"/>
-      <c r="E64" s="92"/>
-      <c r="F64" s="92"/>
-      <c r="G64" s="92"/>
-      <c r="H64" s="92"/>
-      <c r="I64" s="92"/>
-      <c r="J64" s="92"/>
-      <c r="K64" s="92"/>
-      <c r="L64" s="92"/>
-      <c r="M64" s="92"/>
-      <c r="N64" s="92"/>
-      <c r="O64" s="92"/>
+      <c r="B64" s="97"/>
+      <c r="C64" s="97"/>
+      <c r="D64" s="97"/>
+      <c r="E64" s="97"/>
+      <c r="F64" s="97"/>
+      <c r="G64" s="97"/>
+      <c r="H64" s="97"/>
+      <c r="I64" s="97"/>
+      <c r="J64" s="97"/>
+      <c r="K64" s="97"/>
+      <c r="L64" s="97"/>
+      <c r="M64" s="97"/>
+      <c r="N64" s="97"/>
+      <c r="O64" s="97"/>
     </row>
     <row r="65" spans="2:30" ht="17.25">
-      <c r="B65" s="92"/>
-      <c r="C65" s="92"/>
-      <c r="D65" s="92"/>
-      <c r="E65" s="92"/>
-      <c r="F65" s="92"/>
-      <c r="G65" s="92"/>
-      <c r="H65" s="92"/>
-      <c r="I65" s="92"/>
-      <c r="J65" s="92"/>
-      <c r="K65" s="92"/>
-      <c r="L65" s="92"/>
-      <c r="M65" s="92"/>
-      <c r="N65" s="92"/>
-      <c r="O65" s="92"/>
+      <c r="B65" s="97"/>
+      <c r="C65" s="97"/>
+      <c r="D65" s="97"/>
+      <c r="E65" s="97"/>
+      <c r="F65" s="97"/>
+      <c r="G65" s="97"/>
+      <c r="H65" s="97"/>
+      <c r="I65" s="97"/>
+      <c r="J65" s="97"/>
+      <c r="K65" s="97"/>
+      <c r="L65" s="97"/>
+      <c r="M65" s="97"/>
+      <c r="N65" s="97"/>
+      <c r="O65" s="97"/>
       <c r="Q65" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="2:30">
+      <c r="B66" s="97"/>
+      <c r="C66" s="97"/>
+      <c r="D66" s="97"/>
+      <c r="E66" s="97"/>
+      <c r="F66" s="97"/>
+      <c r="G66" s="97"/>
+      <c r="H66" s="97"/>
+      <c r="I66" s="97"/>
+      <c r="J66" s="97"/>
+      <c r="K66" s="97"/>
+      <c r="L66" s="97"/>
+      <c r="M66" s="97"/>
+      <c r="N66" s="97"/>
+      <c r="O66" s="97"/>
+    </row>
+    <row r="67" spans="2:30" ht="15" customHeight="1">
+      <c r="B67" s="96" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" s="96"/>
+      <c r="D67" s="96"/>
+      <c r="E67" s="96"/>
+      <c r="F67" s="96"/>
+      <c r="G67" s="96"/>
+      <c r="H67" s="96"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="96"/>
+      <c r="K67" s="96"/>
+      <c r="L67" s="96"/>
+      <c r="M67" s="96"/>
+      <c r="N67" s="96"/>
+      <c r="O67" s="96"/>
+      <c r="Q67" s="96" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="66" spans="2:30">
-      <c r="B66" s="92"/>
-      <c r="C66" s="92"/>
-      <c r="D66" s="92"/>
-      <c r="E66" s="92"/>
-      <c r="F66" s="92"/>
-      <c r="G66" s="92"/>
-      <c r="H66" s="92"/>
-      <c r="I66" s="92"/>
-      <c r="J66" s="92"/>
-      <c r="K66" s="92"/>
-      <c r="L66" s="92"/>
-      <c r="M66" s="92"/>
-      <c r="N66" s="92"/>
-      <c r="O66" s="92"/>
-    </row>
-    <row r="67" spans="2:30" ht="15" customHeight="1">
-      <c r="B67" s="89" t="s">
-        <v>201</v>
-      </c>
-      <c r="C67" s="89"/>
-      <c r="D67" s="89"/>
-      <c r="E67" s="89"/>
-      <c r="F67" s="89"/>
-      <c r="G67" s="89"/>
-      <c r="H67" s="89"/>
-      <c r="I67" s="89"/>
-      <c r="J67" s="89"/>
-      <c r="K67" s="89"/>
-      <c r="L67" s="89"/>
-      <c r="M67" s="89"/>
-      <c r="N67" s="89"/>
-      <c r="O67" s="89"/>
-      <c r="Q67" s="89" t="s">
-        <v>210</v>
-      </c>
-      <c r="R67" s="89"/>
-      <c r="S67" s="89"/>
-      <c r="T67" s="89"/>
-      <c r="U67" s="89"/>
-      <c r="V67" s="89"/>
-      <c r="W67" s="89"/>
-      <c r="X67" s="89"/>
-      <c r="Y67" s="89"/>
-      <c r="Z67" s="89"/>
-      <c r="AA67" s="89"/>
-      <c r="AB67" s="89"/>
-      <c r="AC67" s="89"/>
-      <c r="AD67" s="89"/>
+      <c r="R67" s="96"/>
+      <c r="S67" s="96"/>
+      <c r="T67" s="96"/>
+      <c r="U67" s="96"/>
+      <c r="V67" s="96"/>
+      <c r="W67" s="96"/>
+      <c r="X67" s="96"/>
+      <c r="Y67" s="96"/>
+      <c r="Z67" s="96"/>
+      <c r="AA67" s="96"/>
+      <c r="AB67" s="96"/>
+      <c r="AC67" s="96"/>
+      <c r="AD67" s="96"/>
     </row>
     <row r="68" spans="2:30">
-      <c r="B68" s="89"/>
-      <c r="C68" s="89"/>
-      <c r="D68" s="89"/>
-      <c r="E68" s="89"/>
-      <c r="F68" s="89"/>
-      <c r="G68" s="89"/>
-      <c r="H68" s="89"/>
-      <c r="I68" s="89"/>
-      <c r="J68" s="89"/>
-      <c r="K68" s="89"/>
-      <c r="L68" s="89"/>
-      <c r="M68" s="89"/>
-      <c r="N68" s="89"/>
-      <c r="O68" s="89"/>
-      <c r="Q68" s="89"/>
-      <c r="R68" s="89"/>
-      <c r="S68" s="89"/>
-      <c r="T68" s="89"/>
-      <c r="U68" s="89"/>
-      <c r="V68" s="89"/>
-      <c r="W68" s="89"/>
-      <c r="X68" s="89"/>
-      <c r="Y68" s="89"/>
-      <c r="Z68" s="89"/>
-      <c r="AA68" s="89"/>
-      <c r="AB68" s="89"/>
-      <c r="AC68" s="89"/>
-      <c r="AD68" s="89"/>
+      <c r="B68" s="96"/>
+      <c r="C68" s="96"/>
+      <c r="D68" s="96"/>
+      <c r="E68" s="96"/>
+      <c r="F68" s="96"/>
+      <c r="G68" s="96"/>
+      <c r="H68" s="96"/>
+      <c r="I68" s="96"/>
+      <c r="J68" s="96"/>
+      <c r="K68" s="96"/>
+      <c r="L68" s="96"/>
+      <c r="M68" s="96"/>
+      <c r="N68" s="96"/>
+      <c r="O68" s="96"/>
+      <c r="Q68" s="96"/>
+      <c r="R68" s="96"/>
+      <c r="S68" s="96"/>
+      <c r="T68" s="96"/>
+      <c r="U68" s="96"/>
+      <c r="V68" s="96"/>
+      <c r="W68" s="96"/>
+      <c r="X68" s="96"/>
+      <c r="Y68" s="96"/>
+      <c r="Z68" s="96"/>
+      <c r="AA68" s="96"/>
+      <c r="AB68" s="96"/>
+      <c r="AC68" s="96"/>
+      <c r="AD68" s="96"/>
     </row>
     <row r="69" spans="2:30">
-      <c r="Q69" s="89"/>
-      <c r="R69" s="89"/>
-      <c r="S69" s="89"/>
-      <c r="T69" s="89"/>
-      <c r="U69" s="89"/>
-      <c r="V69" s="89"/>
-      <c r="W69" s="89"/>
-      <c r="X69" s="89"/>
-      <c r="Y69" s="89"/>
-      <c r="Z69" s="89"/>
-      <c r="AA69" s="89"/>
-      <c r="AB69" s="89"/>
-      <c r="AC69" s="89"/>
-      <c r="AD69" s="89"/>
+      <c r="Q69" s="96"/>
+      <c r="R69" s="96"/>
+      <c r="S69" s="96"/>
+      <c r="T69" s="96"/>
+      <c r="U69" s="96"/>
+      <c r="V69" s="96"/>
+      <c r="W69" s="96"/>
+      <c r="X69" s="96"/>
+      <c r="Y69" s="96"/>
+      <c r="Z69" s="96"/>
+      <c r="AA69" s="96"/>
+      <c r="AB69" s="96"/>
+      <c r="AC69" s="96"/>
+      <c r="AD69" s="96"/>
     </row>
     <row r="70" spans="2:30" ht="17.25">
       <c r="B70" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="2:30" ht="17.25">
@@ -4037,190 +4070,221 @@
       </c>
     </row>
     <row r="73" spans="2:30">
-      <c r="Q73" s="92" t="s">
-        <v>204</v>
-      </c>
-      <c r="R73" s="92"/>
-      <c r="S73" s="92"/>
-      <c r="T73" s="92"/>
-      <c r="U73" s="92"/>
-      <c r="V73" s="92"/>
-      <c r="W73" s="92"/>
-      <c r="X73" s="92"/>
-      <c r="Y73" s="92"/>
-      <c r="Z73" s="92"/>
-      <c r="AA73" s="92"/>
-      <c r="AB73" s="92"/>
-      <c r="AC73" s="92"/>
-      <c r="AD73" s="92"/>
+      <c r="Q73" s="97" t="s">
+        <v>203</v>
+      </c>
+      <c r="R73" s="97"/>
+      <c r="S73" s="97"/>
+      <c r="T73" s="97"/>
+      <c r="U73" s="97"/>
+      <c r="V73" s="97"/>
+      <c r="W73" s="97"/>
+      <c r="X73" s="97"/>
+      <c r="Y73" s="97"/>
+      <c r="Z73" s="97"/>
+      <c r="AA73" s="97"/>
+      <c r="AB73" s="97"/>
+      <c r="AC73" s="97"/>
+      <c r="AD73" s="97"/>
     </row>
     <row r="74" spans="2:30">
-      <c r="Q74" s="92"/>
-      <c r="R74" s="92"/>
-      <c r="S74" s="92"/>
-      <c r="T74" s="92"/>
-      <c r="U74" s="92"/>
-      <c r="V74" s="92"/>
-      <c r="W74" s="92"/>
-      <c r="X74" s="92"/>
-      <c r="Y74" s="92"/>
-      <c r="Z74" s="92"/>
-      <c r="AA74" s="92"/>
-      <c r="AB74" s="92"/>
-      <c r="AC74" s="92"/>
-      <c r="AD74" s="92"/>
+      <c r="Q74" s="97"/>
+      <c r="R74" s="97"/>
+      <c r="S74" s="97"/>
+      <c r="T74" s="97"/>
+      <c r="U74" s="97"/>
+      <c r="V74" s="97"/>
+      <c r="W74" s="97"/>
+      <c r="X74" s="97"/>
+      <c r="Y74" s="97"/>
+      <c r="Z74" s="97"/>
+      <c r="AA74" s="97"/>
+      <c r="AB74" s="97"/>
+      <c r="AC74" s="97"/>
+      <c r="AD74" s="97"/>
     </row>
     <row r="75" spans="2:30" ht="15" customHeight="1">
-      <c r="Q75" s="92"/>
-      <c r="R75" s="92"/>
-      <c r="S75" s="92"/>
-      <c r="T75" s="92"/>
-      <c r="U75" s="92"/>
-      <c r="V75" s="92"/>
-      <c r="W75" s="92"/>
-      <c r="X75" s="92"/>
-      <c r="Y75" s="92"/>
-      <c r="Z75" s="92"/>
-      <c r="AA75" s="92"/>
-      <c r="AB75" s="92"/>
-      <c r="AC75" s="92"/>
-      <c r="AD75" s="92"/>
+      <c r="Q75" s="97"/>
+      <c r="R75" s="97"/>
+      <c r="S75" s="97"/>
+      <c r="T75" s="97"/>
+      <c r="U75" s="97"/>
+      <c r="V75" s="97"/>
+      <c r="W75" s="97"/>
+      <c r="X75" s="97"/>
+      <c r="Y75" s="97"/>
+      <c r="Z75" s="97"/>
+      <c r="AA75" s="97"/>
+      <c r="AB75" s="97"/>
+      <c r="AC75" s="97"/>
+      <c r="AD75" s="97"/>
     </row>
     <row r="76" spans="2:30">
-      <c r="Q76" s="92"/>
-      <c r="R76" s="92"/>
-      <c r="S76" s="92"/>
-      <c r="T76" s="92"/>
-      <c r="U76" s="92"/>
-      <c r="V76" s="92"/>
-      <c r="W76" s="92"/>
-      <c r="X76" s="92"/>
-      <c r="Y76" s="92"/>
-      <c r="Z76" s="92"/>
-      <c r="AA76" s="92"/>
-      <c r="AB76" s="92"/>
-      <c r="AC76" s="92"/>
-      <c r="AD76" s="92"/>
+      <c r="Q76" s="97"/>
+      <c r="R76" s="97"/>
+      <c r="S76" s="97"/>
+      <c r="T76" s="97"/>
+      <c r="U76" s="97"/>
+      <c r="V76" s="97"/>
+      <c r="W76" s="97"/>
+      <c r="X76" s="97"/>
+      <c r="Y76" s="97"/>
+      <c r="Z76" s="97"/>
+      <c r="AA76" s="97"/>
+      <c r="AB76" s="97"/>
+      <c r="AC76" s="97"/>
+      <c r="AD76" s="97"/>
     </row>
     <row r="77" spans="2:30">
-      <c r="Q77" s="92"/>
-      <c r="R77" s="92"/>
-      <c r="S77" s="92"/>
-      <c r="T77" s="92"/>
-      <c r="U77" s="92"/>
-      <c r="V77" s="92"/>
-      <c r="W77" s="92"/>
-      <c r="X77" s="92"/>
-      <c r="Y77" s="92"/>
-      <c r="Z77" s="92"/>
-      <c r="AA77" s="92"/>
-      <c r="AB77" s="92"/>
-      <c r="AC77" s="92"/>
-      <c r="AD77" s="92"/>
+      <c r="Q77" s="97"/>
+      <c r="R77" s="97"/>
+      <c r="S77" s="97"/>
+      <c r="T77" s="97"/>
+      <c r="U77" s="97"/>
+      <c r="V77" s="97"/>
+      <c r="W77" s="97"/>
+      <c r="X77" s="97"/>
+      <c r="Y77" s="97"/>
+      <c r="Z77" s="97"/>
+      <c r="AA77" s="97"/>
+      <c r="AB77" s="97"/>
+      <c r="AC77" s="97"/>
+      <c r="AD77" s="97"/>
     </row>
     <row r="79" spans="2:30" ht="17.25">
-      <c r="B79" s="90" t="s">
+      <c r="B79" s="103" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="90"/>
-      <c r="D79" s="90"/>
-      <c r="E79" s="90"/>
-      <c r="F79" s="90"/>
-      <c r="G79" s="90"/>
-      <c r="H79" s="90"/>
-      <c r="I79" s="90"/>
-      <c r="J79" s="90"/>
-      <c r="K79" s="90"/>
-      <c r="L79" s="90"/>
-      <c r="M79" s="90"/>
-      <c r="N79" s="90"/>
-      <c r="O79" s="90"/>
+      <c r="C79" s="103"/>
+      <c r="D79" s="103"/>
+      <c r="E79" s="103"/>
+      <c r="F79" s="103"/>
+      <c r="G79" s="103"/>
+      <c r="H79" s="103"/>
+      <c r="I79" s="103"/>
+      <c r="J79" s="103"/>
+      <c r="K79" s="103"/>
+      <c r="L79" s="103"/>
+      <c r="M79" s="103"/>
+      <c r="N79" s="103"/>
+      <c r="O79" s="103"/>
       <c r="Q79" s="20" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="81" spans="2:30" ht="15" customHeight="1">
-      <c r="B81" s="89" t="s">
+      <c r="B81" s="96" t="s">
         <v>193</v>
       </c>
-      <c r="C81" s="89"/>
-      <c r="D81" s="89"/>
-      <c r="E81" s="89"/>
-      <c r="F81" s="89"/>
-      <c r="G81" s="89"/>
-      <c r="H81" s="89"/>
-      <c r="I81" s="89"/>
-      <c r="J81" s="89"/>
-      <c r="K81" s="89"/>
-      <c r="L81" s="89"/>
-      <c r="M81" s="89"/>
-      <c r="N81" s="89"/>
-      <c r="O81" s="89"/>
-      <c r="Q81" s="92" t="s">
-        <v>203</v>
-      </c>
-      <c r="R81" s="92"/>
-      <c r="S81" s="92"/>
-      <c r="T81" s="92"/>
-      <c r="U81" s="92"/>
-      <c r="V81" s="92"/>
-      <c r="W81" s="92"/>
-      <c r="X81" s="92"/>
-      <c r="Y81" s="92"/>
-      <c r="Z81" s="92"/>
-      <c r="AA81" s="92"/>
-      <c r="AB81" s="92"/>
-      <c r="AC81" s="92"/>
-      <c r="AD81" s="92"/>
+      <c r="C81" s="96"/>
+      <c r="D81" s="96"/>
+      <c r="E81" s="96"/>
+      <c r="F81" s="96"/>
+      <c r="G81" s="96"/>
+      <c r="H81" s="96"/>
+      <c r="I81" s="96"/>
+      <c r="J81" s="96"/>
+      <c r="K81" s="96"/>
+      <c r="L81" s="96"/>
+      <c r="M81" s="96"/>
+      <c r="N81" s="96"/>
+      <c r="O81" s="96"/>
+      <c r="Q81" s="97" t="s">
+        <v>202</v>
+      </c>
+      <c r="R81" s="97"/>
+      <c r="S81" s="97"/>
+      <c r="T81" s="97"/>
+      <c r="U81" s="97"/>
+      <c r="V81" s="97"/>
+      <c r="W81" s="97"/>
+      <c r="X81" s="97"/>
+      <c r="Y81" s="97"/>
+      <c r="Z81" s="97"/>
+      <c r="AA81" s="97"/>
+      <c r="AB81" s="97"/>
+      <c r="AC81" s="97"/>
+      <c r="AD81" s="97"/>
     </row>
     <row r="82" spans="2:30">
-      <c r="B82" s="89"/>
-      <c r="C82" s="89"/>
-      <c r="D82" s="89"/>
-      <c r="E82" s="89"/>
-      <c r="F82" s="89"/>
-      <c r="G82" s="89"/>
-      <c r="H82" s="89"/>
-      <c r="I82" s="89"/>
-      <c r="J82" s="89"/>
-      <c r="K82" s="89"/>
-      <c r="L82" s="89"/>
-      <c r="M82" s="89"/>
-      <c r="N82" s="89"/>
-      <c r="O82" s="89"/>
-      <c r="Q82" s="92"/>
-      <c r="R82" s="92"/>
-      <c r="S82" s="92"/>
-      <c r="T82" s="92"/>
-      <c r="U82" s="92"/>
-      <c r="V82" s="92"/>
-      <c r="W82" s="92"/>
-      <c r="X82" s="92"/>
-      <c r="Y82" s="92"/>
-      <c r="Z82" s="92"/>
-      <c r="AA82" s="92"/>
-      <c r="AB82" s="92"/>
-      <c r="AC82" s="92"/>
-      <c r="AD82" s="92"/>
+      <c r="B82" s="96"/>
+      <c r="C82" s="96"/>
+      <c r="D82" s="96"/>
+      <c r="E82" s="96"/>
+      <c r="F82" s="96"/>
+      <c r="G82" s="96"/>
+      <c r="H82" s="96"/>
+      <c r="I82" s="96"/>
+      <c r="J82" s="96"/>
+      <c r="K82" s="96"/>
+      <c r="L82" s="96"/>
+      <c r="M82" s="96"/>
+      <c r="N82" s="96"/>
+      <c r="O82" s="96"/>
+      <c r="Q82" s="97"/>
+      <c r="R82" s="97"/>
+      <c r="S82" s="97"/>
+      <c r="T82" s="97"/>
+      <c r="U82" s="97"/>
+      <c r="V82" s="97"/>
+      <c r="W82" s="97"/>
+      <c r="X82" s="97"/>
+      <c r="Y82" s="97"/>
+      <c r="Z82" s="97"/>
+      <c r="AA82" s="97"/>
+      <c r="AB82" s="97"/>
+      <c r="AC82" s="97"/>
+      <c r="AD82" s="97"/>
     </row>
     <row r="83" spans="2:30">
-      <c r="Q83" s="92"/>
-      <c r="R83" s="92"/>
-      <c r="S83" s="92"/>
-      <c r="T83" s="92"/>
-      <c r="U83" s="92"/>
-      <c r="V83" s="92"/>
-      <c r="W83" s="92"/>
-      <c r="X83" s="92"/>
-      <c r="Y83" s="92"/>
-      <c r="Z83" s="92"/>
-      <c r="AA83" s="92"/>
-      <c r="AB83" s="92"/>
-      <c r="AC83" s="92"/>
-      <c r="AD83" s="92"/>
+      <c r="Q83" s="97"/>
+      <c r="R83" s="97"/>
+      <c r="S83" s="97"/>
+      <c r="T83" s="97"/>
+      <c r="U83" s="97"/>
+      <c r="V83" s="97"/>
+      <c r="W83" s="97"/>
+      <c r="X83" s="97"/>
+      <c r="Y83" s="97"/>
+      <c r="Z83" s="97"/>
+      <c r="AA83" s="97"/>
+      <c r="AB83" s="97"/>
+      <c r="AC83" s="97"/>
+      <c r="AD83" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="B38:O39"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="B45:O46"/>
+    <mergeCell ref="B50:O51"/>
+    <mergeCell ref="S42:AB42"/>
+    <mergeCell ref="S45:AB46"/>
+    <mergeCell ref="B55:O56"/>
+    <mergeCell ref="B58:O58"/>
+    <mergeCell ref="B79:O79"/>
+    <mergeCell ref="Q58:AD58"/>
+    <mergeCell ref="B60:O61"/>
+    <mergeCell ref="V48:Z48"/>
+    <mergeCell ref="S50:AB50"/>
+    <mergeCell ref="V40:Z40"/>
+    <mergeCell ref="S29:AB29"/>
+    <mergeCell ref="S26:AB26"/>
+    <mergeCell ref="S33:AB34"/>
+    <mergeCell ref="S37:AB38"/>
+    <mergeCell ref="Q6:AD8"/>
+    <mergeCell ref="Q5:AD5"/>
+    <mergeCell ref="B24:O24"/>
+    <mergeCell ref="B27:O29"/>
+    <mergeCell ref="B31:O32"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="V31:Z31"/>
+    <mergeCell ref="I17:M19"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:O5"/>
+    <mergeCell ref="B8:O9"/>
+    <mergeCell ref="I12:M15"/>
     <mergeCell ref="S52:AB53"/>
     <mergeCell ref="Q67:AD69"/>
     <mergeCell ref="B81:O82"/>
@@ -4229,37 +4293,6 @@
     <mergeCell ref="B67:O68"/>
     <mergeCell ref="Q73:AD77"/>
     <mergeCell ref="Q81:AD83"/>
-    <mergeCell ref="I17:M19"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B4:O5"/>
-    <mergeCell ref="B8:O9"/>
-    <mergeCell ref="I12:M15"/>
-    <mergeCell ref="Q6:AD8"/>
-    <mergeCell ref="Q5:AD5"/>
-    <mergeCell ref="B24:O24"/>
-    <mergeCell ref="B27:O29"/>
-    <mergeCell ref="B31:O32"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="V31:Z31"/>
-    <mergeCell ref="V40:Z40"/>
-    <mergeCell ref="S29:AB29"/>
-    <mergeCell ref="S26:AB26"/>
-    <mergeCell ref="S33:AB34"/>
-    <mergeCell ref="S37:AB38"/>
-    <mergeCell ref="S42:AB42"/>
-    <mergeCell ref="S45:AB46"/>
-    <mergeCell ref="B55:O56"/>
-    <mergeCell ref="B58:O58"/>
-    <mergeCell ref="B79:O79"/>
-    <mergeCell ref="Q58:AD58"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="B38:O39"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B45:O46"/>
-    <mergeCell ref="B50:O51"/>
-    <mergeCell ref="B60:O61"/>
-    <mergeCell ref="V48:Z48"/>
-    <mergeCell ref="S50:AB50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4268,6 +4301,508 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46DDACF-D0ED-4CB1-BA1F-87BB8EEFE26F}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:I40"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="208.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="19.5" thickBot="1">
+      <c r="A1" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="78" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="78" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="78" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" thickTop="1">
+      <c r="A2" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="58">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30">
+      <c r="A3" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75">
+      <c r="A4" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="61">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30">
+      <c r="A5" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="58">
+        <v>0.3</v>
+      </c>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
+      <c r="A8" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="68" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75">
+      <c r="A9" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58">
+        <v>5</v>
+      </c>
+      <c r="F9" s="58">
+        <v>1</v>
+      </c>
+      <c r="G9" s="58">
+        <v>14</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
+      <c r="A10" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="61">
+        <v>14</v>
+      </c>
+      <c r="F10" s="61">
+        <v>6</v>
+      </c>
+      <c r="G10" s="61">
+        <v>41</v>
+      </c>
+      <c r="H10" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="71">
+        <v>20</v>
+      </c>
+      <c r="F11" s="71">
+        <v>10</v>
+      </c>
+      <c r="G11" s="71">
+        <v>41</v>
+      </c>
+      <c r="H11" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30">
+      <c r="A12" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="63"/>
+      <c r="E12" s="71">
+        <v>11.5</v>
+      </c>
+      <c r="F12" s="71">
+        <v>6</v>
+      </c>
+      <c r="G12" s="71">
+        <v>19</v>
+      </c>
+      <c r="H12" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45">
+      <c r="A13" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58">
+        <v>14</v>
+      </c>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45">
+      <c r="A14" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58">
+        <v>21</v>
+      </c>
+      <c r="G14" s="58">
+        <v>42</v>
+      </c>
+      <c r="H14" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
+      <c r="A15" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73">
+        <v>10</v>
+      </c>
+      <c r="F15" s="73">
+        <v>7</v>
+      </c>
+      <c r="G15" s="73">
+        <v>14</v>
+      </c>
+      <c r="H15" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75">
+      <c r="A16" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77">
+        <v>5</v>
+      </c>
+      <c r="F16" s="77">
+        <v>3</v>
+      </c>
+      <c r="G16" s="77">
+        <v>9</v>
+      </c>
+      <c r="H16" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="76" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" ht="18.75">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="18.75">
+      <c r="A19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="B22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+    </row>
+    <row r="40" ht="17.25" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{ED743D3F-91B1-4C36-9B29-97E8F6BA8DEF}"/>
+    <hyperlink ref="I8" r:id="rId2" xr:uid="{1433B300-503C-40E4-8C0F-DD0FA537DAD0}"/>
+    <hyperlink ref="I10" r:id="rId3" xr:uid="{7400FF7B-0CB2-4CB4-98D8-094F6AC3CA8F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E26828-25FC-4634-987C-5618292A93B9}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4276,7 +4811,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
@@ -4294,7 +4829,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="93" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="80">
@@ -4302,7 +4837,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" s="3" customFormat="1">
-      <c r="A3" s="112">
+      <c r="A3" s="94">
         <v>44123</v>
       </c>
       <c r="B3" s="80">
@@ -4310,7 +4845,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" s="3" customFormat="1">
-      <c r="A4" s="111" t="s">
+      <c r="A4" s="93" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="80">
@@ -4318,7 +4853,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" s="3" customFormat="1">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="93" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="80">
@@ -4326,7 +4861,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" s="3" customFormat="1">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="93" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="80">
@@ -4334,7 +4869,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" s="3" customFormat="1">
-      <c r="A7" s="111">
+      <c r="A7" s="93">
         <f>70</f>
         <v>70</v>
       </c>
@@ -4348,7 +4883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC4C435-8BC3-449D-901D-3701FB9529AC}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4368,81 +4903,81 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="C1" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="50" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="109">
+      <c r="B2" s="91">
         <v>64000000</v>
       </c>
-      <c r="C2" s="109">
+      <c r="C2" s="91">
         <v>16000000</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="109">
+      <c r="B3" s="91">
         <v>1920000</v>
       </c>
-      <c r="C3" s="109">
+      <c r="C3" s="91">
         <v>80000</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="108">
+      <c r="B4" s="90">
         <f>B3/B2</f>
         <v>0.03</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="90">
         <f>C3/C2</f>
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="110" t="s">
+      <c r="A5" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="108">
+      <c r="B5" s="90">
         <f>B4/B7</f>
         <v>1.2</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="90">
         <f>C4/B7</f>
         <v>0.19999999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="107"/>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="107" t="s">
-        <v>208</v>
-      </c>
-      <c r="B7" s="108">
+      <c r="A7" s="89" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="90">
         <f>(B3+C3)/(B2+C2)</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C7" s="107"/>
+      <c r="C7" s="89"/>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="8"/>
@@ -4458,7 +4993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A50504-DB74-4372-80E7-81330A036E34}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4484,7 +5019,7 @@
         <v>187</v>
       </c>
       <c r="C1" s="81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1">
@@ -4601,7 +5136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E2194D-F24C-4F86-853D-6FD3370F64B7}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4627,7 +5162,7 @@
         <v>187</v>
       </c>
       <c r="C1" s="81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1">
@@ -4744,7 +5279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D3AC3D-A586-4510-8963-9751795FC8CB}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4878,7 +5413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DAF99A-77C4-4B04-A50C-7585BCDCC48B}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -4981,7 +5516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F8DE8A-8846-4F1C-A15F-BB0A1B1DF3CC}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -5091,7 +5626,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="C6" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5827,7 +6362,7 @@
   <dimension ref="A1:F2725"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -68531,7 +69066,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -71235,6 +71770,490 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B821FE-871F-4FF6-AD12-EEE4379083E0}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="20" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="116" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="117">
+        <v>3780.82191780822</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="116" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="41">
+        <v>0.02</v>
+      </c>
+      <c r="C2">
+        <f>+B2*B1</f>
+        <v>75.616438356164394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A4" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="114" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A5" s="42">
+        <f>Regiones!A2</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="42" t="str">
+        <f>+Regiones!B2</f>
+        <v>Interior de Buenos Aires</v>
+      </c>
+      <c r="C5" s="115">
+        <v>0.27599025234186014</v>
+      </c>
+      <c r="D5" s="113">
+        <f>+C5</f>
+        <v>0.27599025234186014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="42">
+        <f>Regiones!A3</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="42" t="str">
+        <f>+Regiones!B3</f>
+        <v>24 Partidos del Gran Buenos Aires</v>
+      </c>
+      <c r="C6" s="115">
+        <v>0.47945685978820041</v>
+      </c>
+      <c r="D6" s="113">
+        <f>+C6+D5</f>
+        <v>0.75544711213006055</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="42">
+        <f>Regiones!A4</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="42" t="str">
+        <f>+Regiones!B4</f>
+        <v>Córdoba</v>
+      </c>
+      <c r="C7" s="115">
+        <v>3.202898550724638E-2</v>
+      </c>
+      <c r="D7" s="113">
+        <f t="shared" ref="D7:D29" si="0">+C7+D6</f>
+        <v>0.78747609763730697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="42">
+        <f>Regiones!A5</f>
+        <v>4</v>
+      </c>
+      <c r="B8" s="42" t="str">
+        <f>+Regiones!B5</f>
+        <v>Santa Fe</v>
+      </c>
+      <c r="C8" s="115">
+        <v>1.2681159420289856E-2</v>
+      </c>
+      <c r="D8" s="113">
+        <f t="shared" si="0"/>
+        <v>0.80015725705759677</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="42">
+        <f>Regiones!A6</f>
+        <v>5</v>
+      </c>
+      <c r="B9" s="42" t="str">
+        <f>+Regiones!B6</f>
+        <v>Ciudad de Buenos Aires</v>
+      </c>
+      <c r="C9" s="115">
+        <v>0.1397340472902294</v>
+      </c>
+      <c r="D9" s="113">
+        <f t="shared" si="0"/>
+        <v>0.9398913043478262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="42">
+        <f>Regiones!A7</f>
+        <v>6</v>
+      </c>
+      <c r="B10" s="42" t="str">
+        <f>+Regiones!B7</f>
+        <v>Mendoza</v>
+      </c>
+      <c r="C10" s="115">
+        <v>4.4130434782608696E-2</v>
+      </c>
+      <c r="D10" s="113">
+        <f t="shared" si="0"/>
+        <v>0.98402173913043489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="42">
+        <f>Regiones!A8</f>
+        <v>7</v>
+      </c>
+      <c r="B11" s="42" t="str">
+        <f>+Regiones!B8</f>
+        <v>Tucumán</v>
+      </c>
+      <c r="C11" s="115">
+        <v>2.6811594202898552E-3</v>
+      </c>
+      <c r="D11" s="113">
+        <f t="shared" si="0"/>
+        <v>0.98670289855072479</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="42">
+        <f>Regiones!A9</f>
+        <v>8</v>
+      </c>
+      <c r="B12" s="42" t="str">
+        <f>+Regiones!B9</f>
+        <v>Entre Ríos</v>
+      </c>
+      <c r="C12" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D12" s="113">
+        <f t="shared" si="0"/>
+        <v>0.98721980676328513</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="42">
+        <f>Regiones!A10</f>
+        <v>9</v>
+      </c>
+      <c r="B13" s="42" t="str">
+        <f>+Regiones!B10</f>
+        <v>Salta</v>
+      </c>
+      <c r="C13" s="115">
+        <v>2.7536231884057968E-3</v>
+      </c>
+      <c r="D13" s="113">
+        <f t="shared" si="0"/>
+        <v>0.98997342995169091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="42">
+        <f>Regiones!A11</f>
+        <v>10</v>
+      </c>
+      <c r="B14" s="42" t="str">
+        <f>+Regiones!B11</f>
+        <v>Misiones</v>
+      </c>
+      <c r="C14" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D14" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99049033816425125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="42">
+        <f>Regiones!A12</f>
+        <v>11</v>
+      </c>
+      <c r="B15" s="42" t="str">
+        <f>+Regiones!B12</f>
+        <v>Chaco</v>
+      </c>
+      <c r="C15" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D15" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99100724637681159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="42">
+        <f>Regiones!A13</f>
+        <v>12</v>
+      </c>
+      <c r="B16" s="42" t="str">
+        <f>+Regiones!B13</f>
+        <v>Corrientes</v>
+      </c>
+      <c r="C16" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D16" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99152415458937193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="42">
+        <f>Regiones!A14</f>
+        <v>13</v>
+      </c>
+      <c r="B17" s="42" t="str">
+        <f>+Regiones!B14</f>
+        <v>Santiago del Estero</v>
+      </c>
+      <c r="C17" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D17" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99204106280193227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="42">
+        <f>Regiones!A15</f>
+        <v>14</v>
+      </c>
+      <c r="B18" s="42" t="str">
+        <f>+Regiones!B15</f>
+        <v>San Juan</v>
+      </c>
+      <c r="C18" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D18" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99255797101449261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="42">
+        <f>Regiones!A16</f>
+        <v>15</v>
+      </c>
+      <c r="B19" s="42" t="str">
+        <f>+Regiones!B16</f>
+        <v>Jujuy</v>
+      </c>
+      <c r="C19" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D19" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99307487922705295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="42">
+        <f>Regiones!A17</f>
+        <v>16</v>
+      </c>
+      <c r="B20" s="42" t="str">
+        <f>+Regiones!B17</f>
+        <v>Río Negro</v>
+      </c>
+      <c r="C20" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D20" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99359178743961329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="42">
+        <f>Regiones!A18</f>
+        <v>17</v>
+      </c>
+      <c r="B21" s="42" t="str">
+        <f>+Regiones!B18</f>
+        <v>Neuquén</v>
+      </c>
+      <c r="C21" s="115">
+        <v>1.5579710144927536E-3</v>
+      </c>
+      <c r="D21" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99514975845410603</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="42">
+        <f>Regiones!A19</f>
+        <v>18</v>
+      </c>
+      <c r="B22" s="42" t="str">
+        <f>+Regiones!B19</f>
+        <v>Formosa</v>
+      </c>
+      <c r="C22" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D22" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99566666666666637</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="42">
+        <f>Regiones!A20</f>
+        <v>19</v>
+      </c>
+      <c r="B23" s="42" t="str">
+        <f>+Regiones!B20</f>
+        <v>Chubut</v>
+      </c>
+      <c r="C23" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D23" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99618357487922671</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="42">
+        <f>Regiones!A21</f>
+        <v>20</v>
+      </c>
+      <c r="B24" s="42" t="str">
+        <f>+Regiones!B21</f>
+        <v>San Luis</v>
+      </c>
+      <c r="C24" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D24" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99670048309178705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="42">
+        <f>Regiones!A22</f>
+        <v>21</v>
+      </c>
+      <c r="B25" s="42" t="str">
+        <f>+Regiones!B22</f>
+        <v>Catamarca</v>
+      </c>
+      <c r="C25" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D25" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99721739130434739</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="42">
+        <f>Regiones!A23</f>
+        <v>22</v>
+      </c>
+      <c r="B26" s="42" t="str">
+        <f>+Regiones!B23</f>
+        <v>La Rioja</v>
+      </c>
+      <c r="C26" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D26" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99773429951690773</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="42">
+        <f>Regiones!A24</f>
+        <v>23</v>
+      </c>
+      <c r="B27" s="42" t="str">
+        <f>+Regiones!B24</f>
+        <v>La Pampa</v>
+      </c>
+      <c r="C27" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D27" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99825120772946807</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="42">
+        <f>Regiones!A25</f>
+        <v>24</v>
+      </c>
+      <c r="B28" s="42" t="str">
+        <f>+Regiones!B25</f>
+        <v>Santa Cruz</v>
+      </c>
+      <c r="C28" s="115">
+        <v>5.1690821256037041E-4</v>
+      </c>
+      <c r="D28" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99876811594202841</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="42">
+        <f>Regiones!A26</f>
+        <v>25</v>
+      </c>
+      <c r="B29" s="42" t="str">
+        <f>+Regiones!B26</f>
+        <v>Tierra del Fuego</v>
+      </c>
+      <c r="C29" s="115">
+        <v>1.2318840579710144E-3</v>
+      </c>
+      <c r="D29" s="113">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999944</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC2D62F-A7B4-4037-8482-E0DF60B36A90}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
@@ -71243,7 +72262,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
@@ -71258,7 +72277,7 @@
         <v>166</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C1" s="54" t="s">
         <v>167</v>
@@ -71319,7 +72338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B036D3-A03B-46DC-8F79-5557BFA4AF53}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
@@ -71327,7 +72346,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -71350,7 +72369,7 @@
         <v>155</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E1" s="56" t="s">
         <v>156</v>
@@ -71837,7 +72856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F23327-223F-412C-96AA-46EBEDF00338}">
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
@@ -72195,506 +73214,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46DDACF-D0ED-4CB1-BA1F-87BB8EEFE26F}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:I40"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="208.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A1" s="78" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="78" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="78" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="78" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="78" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="78" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" s="78" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" s="78" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="78" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickTop="1">
-      <c r="A2" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="58">
-        <v>0.17899999999999999</v>
-      </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30">
-      <c r="A3" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="63">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="61">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="66" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30">
-      <c r="A5" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="60" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30">
-      <c r="A6" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="60" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30">
-      <c r="A7" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="58">
-        <v>0.3</v>
-      </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="68" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58">
-        <v>5</v>
-      </c>
-      <c r="F9" s="58">
-        <v>1</v>
-      </c>
-      <c r="G9" s="58">
-        <v>14</v>
-      </c>
-      <c r="H9" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="60" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30">
-      <c r="A10" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="61">
-        <v>14</v>
-      </c>
-      <c r="F10" s="61">
-        <v>6</v>
-      </c>
-      <c r="G10" s="61">
-        <v>41</v>
-      </c>
-      <c r="H10" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30">
-      <c r="A11" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="71">
-        <v>20</v>
-      </c>
-      <c r="F11" s="71">
-        <v>10</v>
-      </c>
-      <c r="G11" s="71">
-        <v>41</v>
-      </c>
-      <c r="H11" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30">
-      <c r="A12" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="71">
-        <v>11.5</v>
-      </c>
-      <c r="F12" s="71">
-        <v>6</v>
-      </c>
-      <c r="G12" s="71">
-        <v>19</v>
-      </c>
-      <c r="H12" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45">
-      <c r="A13" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58">
-        <v>14</v>
-      </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="60" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45">
-      <c r="A14" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58">
-        <v>21</v>
-      </c>
-      <c r="G14" s="58">
-        <v>42</v>
-      </c>
-      <c r="H14" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="60" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30">
-      <c r="A15" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="70" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73">
-        <v>10</v>
-      </c>
-      <c r="F15" s="73">
-        <v>7</v>
-      </c>
-      <c r="G15" s="73">
-        <v>14</v>
-      </c>
-      <c r="H15" s="73" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="74" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75">
-      <c r="A16" s="75" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77">
-        <v>5</v>
-      </c>
-      <c r="F16" s="77">
-        <v>3</v>
-      </c>
-      <c r="G16" s="77">
-        <v>9</v>
-      </c>
-      <c r="H16" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="76" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" ht="18.75">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="18.75">
-      <c r="A19" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="B22" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-    </row>
-    <row r="40" ht="17.25" customHeight="1"/>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{ED743D3F-91B1-4C36-9B29-97E8F6BA8DEF}"/>
-    <hyperlink ref="I8" r:id="rId2" xr:uid="{1433B300-503C-40E4-8C0F-DD0FA537DAD0}"/>
-    <hyperlink ref="I10" r:id="rId3" xr:uid="{7400FF7B-0CB2-4CB4-98D8-094F6AC3CA8F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added Custom Policy & Closing External Trips options
</commit_message>
<xml_diff>
--- a/COVID Contagio Argentina Monte Carlo/Input/Input_Simulador.xlsx
+++ b/COVID Contagio Argentina Monte Carlo/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina Monte Carlo\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A46AA0-5390-4146-AF2B-8CAED59DD7EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442AFCD7-AA7C-4EDE-811B-B126B37AB8E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15750" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15750" activeTab="5" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="28" r:id="rId1"/>
@@ -2252,11 +2252,32 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2267,16 +2288,10 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2288,22 +2303,7 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2744,8 +2744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFB5D56-B68E-4E9D-9EC4-1DBA7AFCA152}">
   <dimension ref="A1:AS83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2758,22 +2758,22 @@
   <sheetData>
     <row r="1" spans="2:45" s="9" customFormat="1"/>
     <row r="2" spans="2:45" s="9" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="110" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -2791,248 +2791,248 @@
     </row>
     <row r="3" spans="2:45" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:45" ht="15" customHeight="1">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="106" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+      <c r="O4" s="106"/>
     </row>
     <row r="5" spans="2:45" ht="22.5" customHeight="1">
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="101"/>
-      <c r="N5" s="101"/>
-      <c r="O5" s="101"/>
-      <c r="Q5" s="108" t="s">
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="Q5" s="114" t="s">
         <v>173</v>
       </c>
-      <c r="R5" s="108"/>
-      <c r="S5" s="108"/>
-      <c r="T5" s="108"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="108"/>
-      <c r="W5" s="108"/>
-      <c r="X5" s="108"/>
-      <c r="Y5" s="108"/>
-      <c r="Z5" s="108"/>
-      <c r="AA5" s="108"/>
-      <c r="AB5" s="108"/>
-      <c r="AC5" s="108"/>
-      <c r="AD5" s="108"/>
+      <c r="R5" s="114"/>
+      <c r="S5" s="114"/>
+      <c r="T5" s="114"/>
+      <c r="U5" s="114"/>
+      <c r="V5" s="114"/>
+      <c r="W5" s="114"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="114"/>
+      <c r="Z5" s="114"/>
+      <c r="AA5" s="114"/>
+      <c r="AB5" s="114"/>
+      <c r="AC5" s="114"/>
+      <c r="AD5" s="114"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
     </row>
     <row r="6" spans="2:45">
-      <c r="Q6" s="107" t="s">
+      <c r="Q6" s="113" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="107"/>
-      <c r="AA6" s="107"/>
-      <c r="AB6" s="107"/>
-      <c r="AC6" s="107"/>
-      <c r="AD6" s="107"/>
+      <c r="R6" s="113"/>
+      <c r="S6" s="113"/>
+      <c r="T6" s="113"/>
+      <c r="U6" s="113"/>
+      <c r="V6" s="113"/>
+      <c r="W6" s="113"/>
+      <c r="X6" s="113"/>
+      <c r="Y6" s="113"/>
+      <c r="Z6" s="113"/>
+      <c r="AA6" s="113"/>
+      <c r="AB6" s="113"/>
+      <c r="AC6" s="113"/>
+      <c r="AD6" s="113"/>
     </row>
     <row r="7" spans="2:45">
-      <c r="Q7" s="107"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="107"/>
-      <c r="AB7" s="107"/>
-      <c r="AC7" s="107"/>
-      <c r="AD7" s="107"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="113"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="113"/>
+      <c r="V7" s="113"/>
+      <c r="W7" s="113"/>
+      <c r="X7" s="113"/>
+      <c r="Y7" s="113"/>
+      <c r="Z7" s="113"/>
+      <c r="AA7" s="113"/>
+      <c r="AB7" s="113"/>
+      <c r="AC7" s="113"/>
+      <c r="AD7" s="113"/>
     </row>
     <row r="8" spans="2:45" ht="15" customHeight="1">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="101"/>
-      <c r="Q8" s="107"/>
-      <c r="R8" s="107"/>
-      <c r="S8" s="107"/>
-      <c r="T8" s="107"/>
-      <c r="U8" s="107"/>
-      <c r="V8" s="107"/>
-      <c r="W8" s="107"/>
-      <c r="X8" s="107"/>
-      <c r="Y8" s="107"/>
-      <c r="Z8" s="107"/>
-      <c r="AA8" s="107"/>
-      <c r="AB8" s="107"/>
-      <c r="AC8" s="107"/>
-      <c r="AD8" s="107"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="106"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="106"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="106"/>
+      <c r="O8" s="106"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
+      <c r="Y8" s="113"/>
+      <c r="Z8" s="113"/>
+      <c r="AA8" s="113"/>
+      <c r="AB8" s="113"/>
+      <c r="AC8" s="113"/>
+      <c r="AD8" s="113"/>
     </row>
     <row r="9" spans="2:45" ht="17.25" customHeight="1">
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
+      <c r="B9" s="106"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="106"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="106"/>
+      <c r="I9" s="106"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="106"/>
+      <c r="M9" s="106"/>
+      <c r="N9" s="106"/>
+      <c r="O9" s="106"/>
     </row>
     <row r="12" spans="2:45" ht="17.25" customHeight="1">
       <c r="D12" s="15" t="s">
         <v>96</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="104" t="s">
+      <c r="I12" s="111" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105"/>
-      <c r="M12" s="105"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="112"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
     </row>
     <row r="13" spans="2:45" ht="17.25">
       <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
     </row>
     <row r="14" spans="2:45" ht="17.25">
       <c r="D14" s="13" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="112"/>
+      <c r="K14" s="112"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="112"/>
     </row>
     <row r="15" spans="2:45" ht="17.25" customHeight="1">
       <c r="D15" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="104"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
     </row>
     <row r="17" spans="2:43" ht="17.25" customHeight="1">
       <c r="G17" s="18"/>
-      <c r="I17" s="104" t="s">
+      <c r="I17" s="111" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="105"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="112"/>
+      <c r="L17" s="112"/>
+      <c r="M17" s="112"/>
     </row>
     <row r="18" spans="2:43" ht="17.25">
       <c r="D18" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="104"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+      <c r="M18" s="112"/>
     </row>
     <row r="19" spans="2:43" ht="15" customHeight="1">
-      <c r="I19" s="104"/>
-      <c r="J19" s="105"/>
-      <c r="K19" s="105"/>
-      <c r="L19" s="105"/>
-      <c r="M19" s="105"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="112"/>
+      <c r="L19" s="112"/>
+      <c r="M19" s="112"/>
     </row>
     <row r="22" spans="2:43">
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="115" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="110"/>
-      <c r="M22" s="110"/>
-      <c r="N22" s="110"/>
-      <c r="O22" s="110"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="115"/>
+      <c r="K22" s="115"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="115"/>
+      <c r="O22" s="115"/>
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1"/>
     <row r="24" spans="2:43" ht="17.25">
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="101" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="109"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="109"/>
-      <c r="M24" s="109"/>
-      <c r="N24" s="109"/>
-      <c r="O24" s="109"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="101"/>
+      <c r="H24" s="101"/>
+      <c r="I24" s="101"/>
+      <c r="J24" s="101"/>
+      <c r="K24" s="101"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="101"/>
+      <c r="N24" s="101"/>
+      <c r="O24" s="101"/>
     </row>
     <row r="25" spans="2:43">
       <c r="R25" s="23"/>
@@ -3053,37 +3053,37 @@
         <v>96</v>
       </c>
       <c r="R26" s="26"/>
-      <c r="S26" s="114" t="s">
+      <c r="S26" s="118" t="s">
         <v>106</v>
       </c>
-      <c r="T26" s="114"/>
-      <c r="U26" s="114"/>
-      <c r="V26" s="114"/>
-      <c r="W26" s="114"/>
-      <c r="X26" s="114"/>
-      <c r="Y26" s="114"/>
-      <c r="Z26" s="114"/>
-      <c r="AA26" s="114"/>
-      <c r="AB26" s="114"/>
+      <c r="T26" s="118"/>
+      <c r="U26" s="118"/>
+      <c r="V26" s="118"/>
+      <c r="W26" s="118"/>
+      <c r="X26" s="118"/>
+      <c r="Y26" s="118"/>
+      <c r="Z26" s="118"/>
+      <c r="AA26" s="118"/>
+      <c r="AB26" s="118"/>
       <c r="AC26" s="27"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1">
-      <c r="B27" s="101" t="s">
+      <c r="B27" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
-      <c r="M27" s="101"/>
-      <c r="N27" s="101"/>
-      <c r="O27" s="101"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="106"/>
+      <c r="M27" s="106"/>
+      <c r="N27" s="106"/>
+      <c r="O27" s="106"/>
       <c r="R27" s="26"/>
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
@@ -3108,51 +3108,51 @@
       <c r="AQ27" s="18"/>
     </row>
     <row r="28" spans="2:43" ht="15" customHeight="1">
-      <c r="B28" s="101"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="101"/>
-      <c r="I28" s="101"/>
-      <c r="J28" s="101"/>
-      <c r="K28" s="101"/>
-      <c r="L28" s="101"/>
-      <c r="M28" s="101"/>
-      <c r="N28" s="101"/>
-      <c r="O28" s="101"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="106"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="106"/>
+      <c r="I28" s="106"/>
+      <c r="J28" s="106"/>
+      <c r="K28" s="106"/>
+      <c r="L28" s="106"/>
+      <c r="M28" s="106"/>
+      <c r="N28" s="106"/>
+      <c r="O28" s="106"/>
       <c r="R28" s="26"/>
       <c r="AC28" s="27"/>
     </row>
     <row r="29" spans="2:43" ht="17.25">
-      <c r="B29" s="101"/>
-      <c r="C29" s="101"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
-      <c r="J29" s="101"/>
-      <c r="K29" s="101"/>
-      <c r="L29" s="101"/>
-      <c r="M29" s="101"/>
-      <c r="N29" s="101"/>
-      <c r="O29" s="101"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="106"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="106"/>
+      <c r="H29" s="106"/>
+      <c r="I29" s="106"/>
+      <c r="J29" s="106"/>
+      <c r="K29" s="106"/>
+      <c r="L29" s="106"/>
+      <c r="M29" s="106"/>
+      <c r="N29" s="106"/>
+      <c r="O29" s="106"/>
       <c r="R29" s="26"/>
-      <c r="S29" s="113" t="s">
+      <c r="S29" s="109" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="113"/>
-      <c r="U29" s="113"/>
-      <c r="V29" s="113"/>
-      <c r="W29" s="113"/>
-      <c r="X29" s="113"/>
-      <c r="Y29" s="113"/>
-      <c r="Z29" s="113"/>
-      <c r="AA29" s="113"/>
-      <c r="AB29" s="113"/>
+      <c r="T29" s="109"/>
+      <c r="U29" s="109"/>
+      <c r="V29" s="109"/>
+      <c r="W29" s="109"/>
+      <c r="X29" s="109"/>
+      <c r="Y29" s="109"/>
+      <c r="Z29" s="109"/>
+      <c r="AA29" s="109"/>
+      <c r="AB29" s="109"/>
       <c r="AC29" s="27"/>
     </row>
     <row r="30" spans="2:43">
@@ -3170,52 +3170,52 @@
       <c r="AC30" s="27"/>
     </row>
     <row r="31" spans="2:43" ht="17.25">
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101"/>
-      <c r="I31" s="101"/>
-      <c r="J31" s="101"/>
-      <c r="K31" s="101"/>
-      <c r="L31" s="101"/>
-      <c r="M31" s="101"/>
-      <c r="N31" s="101"/>
-      <c r="O31" s="101"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="106"/>
+      <c r="J31" s="106"/>
+      <c r="K31" s="106"/>
+      <c r="L31" s="106"/>
+      <c r="M31" s="106"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="106"/>
       <c r="R31" s="26"/>
       <c r="S31" s="18"/>
       <c r="T31" s="18"/>
       <c r="U31" s="18"/>
-      <c r="V31" s="111" t="s">
+      <c r="V31" s="116" t="s">
         <v>109</v>
       </c>
-      <c r="W31" s="111"/>
-      <c r="X31" s="111"/>
-      <c r="Y31" s="111"/>
-      <c r="Z31" s="111"/>
+      <c r="W31" s="116"/>
+      <c r="X31" s="116"/>
+      <c r="Y31" s="116"/>
+      <c r="Z31" s="116"/>
       <c r="AA31" s="18"/>
       <c r="AB31" s="18"/>
       <c r="AC31" s="27"/>
     </row>
     <row r="32" spans="2:43" ht="15" customHeight="1">
-      <c r="B32" s="101"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="101"/>
-      <c r="G32" s="101"/>
-      <c r="H32" s="101"/>
-      <c r="I32" s="101"/>
-      <c r="J32" s="101"/>
-      <c r="K32" s="101"/>
-      <c r="L32" s="101"/>
-      <c r="M32" s="101"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
+      <c r="B32" s="106"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="106"/>
+      <c r="E32" s="106"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="106"/>
+      <c r="H32" s="106"/>
+      <c r="I32" s="106"/>
+      <c r="J32" s="106"/>
+      <c r="K32" s="106"/>
+      <c r="L32" s="106"/>
+      <c r="M32" s="106"/>
+      <c r="N32" s="106"/>
+      <c r="O32" s="106"/>
       <c r="R32" s="26"/>
       <c r="S32" s="18"/>
       <c r="T32" s="18"/>
@@ -3230,61 +3230,61 @@
       <c r="AC32" s="27"/>
     </row>
     <row r="33" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B33" s="101" t="s">
+      <c r="B33" s="106" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="101"/>
-      <c r="H33" s="101"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="101"/>
-      <c r="K33" s="101"/>
-      <c r="L33" s="101"/>
-      <c r="M33" s="101"/>
-      <c r="N33" s="101"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="106"/>
+      <c r="I33" s="106"/>
+      <c r="J33" s="106"/>
+      <c r="K33" s="106"/>
+      <c r="L33" s="106"/>
+      <c r="M33" s="106"/>
+      <c r="N33" s="106"/>
       <c r="R33" s="26"/>
-      <c r="S33" s="115" t="s">
+      <c r="S33" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="115"/>
-      <c r="U33" s="115"/>
-      <c r="V33" s="115"/>
-      <c r="W33" s="115"/>
-      <c r="X33" s="115"/>
-      <c r="Y33" s="115"/>
-      <c r="Z33" s="115"/>
-      <c r="AA33" s="115"/>
-      <c r="AB33" s="115"/>
+      <c r="T33" s="107"/>
+      <c r="U33" s="107"/>
+      <c r="V33" s="107"/>
+      <c r="W33" s="107"/>
+      <c r="X33" s="107"/>
+      <c r="Y33" s="107"/>
+      <c r="Z33" s="107"/>
+      <c r="AA33" s="107"/>
+      <c r="AB33" s="107"/>
       <c r="AC33" s="27"/>
     </row>
     <row r="34" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B34" s="101"/>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
-      <c r="L34" s="101"/>
-      <c r="M34" s="101"/>
-      <c r="N34" s="101"/>
+      <c r="B34" s="106"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="106"/>
+      <c r="F34" s="106"/>
+      <c r="G34" s="106"/>
+      <c r="H34" s="106"/>
+      <c r="I34" s="106"/>
+      <c r="J34" s="106"/>
+      <c r="K34" s="106"/>
+      <c r="L34" s="106"/>
+      <c r="M34" s="106"/>
+      <c r="N34" s="106"/>
       <c r="R34" s="26"/>
-      <c r="S34" s="115"/>
-      <c r="T34" s="115"/>
-      <c r="U34" s="115"/>
-      <c r="V34" s="115"/>
-      <c r="W34" s="115"/>
-      <c r="X34" s="115"/>
-      <c r="Y34" s="115"/>
-      <c r="Z34" s="115"/>
-      <c r="AA34" s="115"/>
-      <c r="AB34" s="115"/>
+      <c r="S34" s="107"/>
+      <c r="T34" s="107"/>
+      <c r="U34" s="107"/>
+      <c r="V34" s="107"/>
+      <c r="W34" s="107"/>
+      <c r="X34" s="107"/>
+      <c r="Y34" s="107"/>
+      <c r="Z34" s="107"/>
+      <c r="AA34" s="107"/>
+      <c r="AB34" s="107"/>
       <c r="AC34" s="27"/>
     </row>
     <row r="35" spans="2:32">
@@ -3322,67 +3322,67 @@
     </row>
     <row r="37" spans="2:32">
       <c r="R37" s="26"/>
-      <c r="S37" s="116" t="s">
+      <c r="S37" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="T37" s="116"/>
-      <c r="U37" s="116"/>
-      <c r="V37" s="116"/>
-      <c r="W37" s="116"/>
-      <c r="X37" s="116"/>
-      <c r="Y37" s="116"/>
-      <c r="Z37" s="116"/>
-      <c r="AA37" s="116"/>
-      <c r="AB37" s="116"/>
+      <c r="T37" s="108"/>
+      <c r="U37" s="108"/>
+      <c r="V37" s="108"/>
+      <c r="W37" s="108"/>
+      <c r="X37" s="108"/>
+      <c r="Y37" s="108"/>
+      <c r="Z37" s="108"/>
+      <c r="AA37" s="108"/>
+      <c r="AB37" s="108"/>
       <c r="AC37" s="27"/>
       <c r="AF37" s="9"/>
     </row>
     <row r="38" spans="2:32">
-      <c r="B38" s="101" t="s">
+      <c r="B38" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="101"/>
-      <c r="M38" s="101"/>
-      <c r="N38" s="101"/>
-      <c r="O38" s="101"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="106"/>
+      <c r="K38" s="106"/>
+      <c r="L38" s="106"/>
+      <c r="M38" s="106"/>
+      <c r="N38" s="106"/>
+      <c r="O38" s="106"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="116"/>
-      <c r="T38" s="116"/>
-      <c r="U38" s="116"/>
-      <c r="V38" s="116"/>
-      <c r="W38" s="116"/>
-      <c r="X38" s="116"/>
-      <c r="Y38" s="116"/>
-      <c r="Z38" s="116"/>
-      <c r="AA38" s="116"/>
-      <c r="AB38" s="116"/>
+      <c r="S38" s="108"/>
+      <c r="T38" s="108"/>
+      <c r="U38" s="108"/>
+      <c r="V38" s="108"/>
+      <c r="W38" s="108"/>
+      <c r="X38" s="108"/>
+      <c r="Y38" s="108"/>
+      <c r="Z38" s="108"/>
+      <c r="AA38" s="108"/>
+      <c r="AB38" s="108"/>
       <c r="AC38" s="27"/>
       <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="2:32">
-      <c r="B39" s="101"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="101"/>
-      <c r="F39" s="101"/>
-      <c r="G39" s="101"/>
-      <c r="H39" s="101"/>
-      <c r="I39" s="101"/>
-      <c r="J39" s="101"/>
-      <c r="K39" s="101"/>
-      <c r="L39" s="101"/>
-      <c r="M39" s="101"/>
-      <c r="N39" s="101"/>
-      <c r="O39" s="101"/>
+      <c r="B39" s="106"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="106"/>
+      <c r="I39" s="106"/>
+      <c r="J39" s="106"/>
+      <c r="K39" s="106"/>
+      <c r="L39" s="106"/>
+      <c r="M39" s="106"/>
+      <c r="N39" s="106"/>
+      <c r="O39" s="106"/>
       <c r="R39" s="26"/>
       <c r="S39" s="18"/>
       <c r="T39" s="19"/>
@@ -3402,34 +3402,34 @@
       <c r="S40" s="18"/>
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
-      <c r="V40" s="112" t="s">
+      <c r="V40" s="117" t="s">
         <v>110</v>
       </c>
-      <c r="W40" s="112"/>
-      <c r="X40" s="112"/>
-      <c r="Y40" s="112"/>
-      <c r="Z40" s="112"/>
+      <c r="W40" s="117"/>
+      <c r="X40" s="117"/>
+      <c r="Y40" s="117"/>
+      <c r="Z40" s="117"/>
       <c r="AA40" s="19"/>
       <c r="AB40" s="19"/>
       <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="2:32" ht="17.25">
-      <c r="B41" s="109" t="s">
+      <c r="B41" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="109"/>
-      <c r="D41" s="109"/>
-      <c r="E41" s="109"/>
-      <c r="F41" s="109"/>
-      <c r="G41" s="109"/>
-      <c r="H41" s="109"/>
-      <c r="I41" s="109"/>
-      <c r="J41" s="109"/>
-      <c r="K41" s="109"/>
-      <c r="L41" s="109"/>
-      <c r="M41" s="109"/>
-      <c r="N41" s="109"/>
-      <c r="O41" s="109"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="101"/>
+      <c r="E41" s="101"/>
+      <c r="F41" s="101"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="101"/>
+      <c r="J41" s="101"/>
+      <c r="K41" s="101"/>
+      <c r="L41" s="101"/>
+      <c r="M41" s="101"/>
+      <c r="N41" s="101"/>
+      <c r="O41" s="101"/>
       <c r="R41" s="26"/>
       <c r="S41" s="18"/>
       <c r="T41" s="18"/>
@@ -3445,18 +3445,18 @@
     </row>
     <row r="42" spans="2:32" ht="17.25">
       <c r="R42" s="26"/>
-      <c r="S42" s="113" t="s">
+      <c r="S42" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="T42" s="113"/>
-      <c r="U42" s="113"/>
-      <c r="V42" s="113"/>
-      <c r="W42" s="113"/>
-      <c r="X42" s="113"/>
-      <c r="Y42" s="113"/>
-      <c r="Z42" s="113"/>
-      <c r="AA42" s="113"/>
-      <c r="AB42" s="113"/>
+      <c r="T42" s="109"/>
+      <c r="U42" s="109"/>
+      <c r="V42" s="109"/>
+      <c r="W42" s="109"/>
+      <c r="X42" s="109"/>
+      <c r="Y42" s="109"/>
+      <c r="Z42" s="109"/>
+      <c r="AA42" s="109"/>
+      <c r="AB42" s="109"/>
       <c r="AC42" s="27"/>
     </row>
     <row r="43" spans="2:32" ht="17.25">
@@ -3491,63 +3491,63 @@
       <c r="AC44" s="27"/>
     </row>
     <row r="45" spans="2:32">
-      <c r="B45" s="101" t="s">
+      <c r="B45" s="106" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="101"/>
-      <c r="D45" s="101"/>
-      <c r="E45" s="101"/>
-      <c r="F45" s="101"/>
-      <c r="G45" s="101"/>
-      <c r="H45" s="101"/>
-      <c r="I45" s="101"/>
-      <c r="J45" s="101"/>
-      <c r="K45" s="101"/>
-      <c r="L45" s="101"/>
-      <c r="M45" s="101"/>
-      <c r="N45" s="101"/>
-      <c r="O45" s="101"/>
+      <c r="C45" s="106"/>
+      <c r="D45" s="106"/>
+      <c r="E45" s="106"/>
+      <c r="F45" s="106"/>
+      <c r="G45" s="106"/>
+      <c r="H45" s="106"/>
+      <c r="I45" s="106"/>
+      <c r="J45" s="106"/>
+      <c r="K45" s="106"/>
+      <c r="L45" s="106"/>
+      <c r="M45" s="106"/>
+      <c r="N45" s="106"/>
+      <c r="O45" s="106"/>
       <c r="R45" s="26"/>
-      <c r="S45" s="115" t="s">
+      <c r="S45" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="T45" s="115"/>
-      <c r="U45" s="115"/>
-      <c r="V45" s="115"/>
-      <c r="W45" s="115"/>
-      <c r="X45" s="115"/>
-      <c r="Y45" s="115"/>
-      <c r="Z45" s="115"/>
-      <c r="AA45" s="115"/>
-      <c r="AB45" s="115"/>
+      <c r="T45" s="107"/>
+      <c r="U45" s="107"/>
+      <c r="V45" s="107"/>
+      <c r="W45" s="107"/>
+      <c r="X45" s="107"/>
+      <c r="Y45" s="107"/>
+      <c r="Z45" s="107"/>
+      <c r="AA45" s="107"/>
+      <c r="AB45" s="107"/>
       <c r="AC45" s="27"/>
     </row>
     <row r="46" spans="2:32" ht="15" customHeight="1">
-      <c r="B46" s="101"/>
-      <c r="C46" s="101"/>
-      <c r="D46" s="101"/>
-      <c r="E46" s="101"/>
-      <c r="F46" s="101"/>
-      <c r="G46" s="101"/>
-      <c r="H46" s="101"/>
-      <c r="I46" s="101"/>
-      <c r="J46" s="101"/>
-      <c r="K46" s="101"/>
-      <c r="L46" s="101"/>
-      <c r="M46" s="101"/>
-      <c r="N46" s="101"/>
-      <c r="O46" s="101"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="106"/>
+      <c r="E46" s="106"/>
+      <c r="F46" s="106"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="106"/>
+      <c r="I46" s="106"/>
+      <c r="J46" s="106"/>
+      <c r="K46" s="106"/>
+      <c r="L46" s="106"/>
+      <c r="M46" s="106"/>
+      <c r="N46" s="106"/>
+      <c r="O46" s="106"/>
       <c r="R46" s="26"/>
-      <c r="S46" s="115"/>
-      <c r="T46" s="115"/>
-      <c r="U46" s="115"/>
-      <c r="V46" s="115"/>
-      <c r="W46" s="115"/>
-      <c r="X46" s="115"/>
-      <c r="Y46" s="115"/>
-      <c r="Z46" s="115"/>
-      <c r="AA46" s="115"/>
-      <c r="AB46" s="115"/>
+      <c r="S46" s="107"/>
+      <c r="T46" s="107"/>
+      <c r="U46" s="107"/>
+      <c r="V46" s="107"/>
+      <c r="W46" s="107"/>
+      <c r="X46" s="107"/>
+      <c r="Y46" s="107"/>
+      <c r="Z46" s="107"/>
+      <c r="AA46" s="107"/>
+      <c r="AB46" s="107"/>
       <c r="AC46" s="27"/>
     </row>
     <row r="47" spans="2:32" ht="15" customHeight="1">
@@ -3572,13 +3572,13 @@
       <c r="S48" s="18"/>
       <c r="T48" s="18"/>
       <c r="U48" s="18"/>
-      <c r="V48" s="118" t="s">
+      <c r="V48" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="W48" s="118"/>
-      <c r="X48" s="118"/>
-      <c r="Y48" s="118"/>
-      <c r="Z48" s="118"/>
+      <c r="W48" s="104"/>
+      <c r="X48" s="104"/>
+      <c r="Y48" s="104"/>
+      <c r="Z48" s="104"/>
       <c r="AA48" s="18"/>
       <c r="AB48" s="18"/>
       <c r="AC48" s="27"/>
@@ -3598,52 +3598,52 @@
       <c r="AC49" s="27"/>
     </row>
     <row r="50" spans="2:43">
-      <c r="B50" s="101" t="s">
+      <c r="B50" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="101"/>
-      <c r="D50" s="101"/>
-      <c r="E50" s="101"/>
-      <c r="F50" s="101"/>
-      <c r="G50" s="101"/>
-      <c r="H50" s="101"/>
-      <c r="I50" s="101"/>
-      <c r="J50" s="101"/>
-      <c r="K50" s="101"/>
-      <c r="L50" s="101"/>
-      <c r="M50" s="101"/>
-      <c r="N50" s="101"/>
-      <c r="O50" s="101"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="106"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="106"/>
+      <c r="H50" s="106"/>
+      <c r="I50" s="106"/>
+      <c r="J50" s="106"/>
+      <c r="K50" s="106"/>
+      <c r="L50" s="106"/>
+      <c r="M50" s="106"/>
+      <c r="N50" s="106"/>
+      <c r="O50" s="106"/>
       <c r="R50" s="26"/>
-      <c r="S50" s="106" t="s">
+      <c r="S50" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="T50" s="106"/>
-      <c r="U50" s="106"/>
-      <c r="V50" s="106"/>
-      <c r="W50" s="106"/>
-      <c r="X50" s="106"/>
-      <c r="Y50" s="106"/>
-      <c r="Z50" s="106"/>
-      <c r="AA50" s="106"/>
-      <c r="AB50" s="106"/>
+      <c r="T50" s="105"/>
+      <c r="U50" s="105"/>
+      <c r="V50" s="105"/>
+      <c r="W50" s="105"/>
+      <c r="X50" s="105"/>
+      <c r="Y50" s="105"/>
+      <c r="Z50" s="105"/>
+      <c r="AA50" s="105"/>
+      <c r="AB50" s="105"/>
       <c r="AC50" s="27"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1">
-      <c r="B51" s="101"/>
-      <c r="C51" s="101"/>
-      <c r="D51" s="101"/>
-      <c r="E51" s="101"/>
-      <c r="F51" s="101"/>
-      <c r="G51" s="101"/>
-      <c r="H51" s="101"/>
-      <c r="I51" s="101"/>
-      <c r="J51" s="101"/>
-      <c r="K51" s="101"/>
-      <c r="L51" s="101"/>
-      <c r="M51" s="101"/>
-      <c r="N51" s="101"/>
-      <c r="O51" s="101"/>
+      <c r="B51" s="106"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="106"/>
+      <c r="E51" s="106"/>
+      <c r="F51" s="106"/>
+      <c r="G51" s="106"/>
+      <c r="H51" s="106"/>
+      <c r="I51" s="106"/>
+      <c r="J51" s="106"/>
+      <c r="K51" s="106"/>
+      <c r="L51" s="106"/>
+      <c r="M51" s="106"/>
+      <c r="N51" s="106"/>
+      <c r="O51" s="106"/>
       <c r="R51" s="26"/>
       <c r="S51" s="18"/>
       <c r="T51" s="18"/>
@@ -3659,18 +3659,18 @@
     </row>
     <row r="52" spans="2:43">
       <c r="R52" s="26"/>
-      <c r="S52" s="106" t="s">
+      <c r="S52" s="105" t="s">
         <v>116</v>
       </c>
-      <c r="T52" s="106"/>
-      <c r="U52" s="106"/>
-      <c r="V52" s="106"/>
-      <c r="W52" s="106"/>
-      <c r="X52" s="106"/>
-      <c r="Y52" s="106"/>
-      <c r="Z52" s="106"/>
-      <c r="AA52" s="106"/>
-      <c r="AB52" s="106"/>
+      <c r="T52" s="105"/>
+      <c r="U52" s="105"/>
+      <c r="V52" s="105"/>
+      <c r="W52" s="105"/>
+      <c r="X52" s="105"/>
+      <c r="Y52" s="105"/>
+      <c r="Z52" s="105"/>
+      <c r="AA52" s="105"/>
+      <c r="AB52" s="105"/>
       <c r="AC52" s="27"/>
     </row>
     <row r="53" spans="2:43" ht="15.75" customHeight="1">
@@ -3678,16 +3678,16 @@
         <v>147</v>
       </c>
       <c r="R53" s="26"/>
-      <c r="S53" s="106"/>
-      <c r="T53" s="106"/>
-      <c r="U53" s="106"/>
-      <c r="V53" s="106"/>
-      <c r="W53" s="106"/>
-      <c r="X53" s="106"/>
-      <c r="Y53" s="106"/>
-      <c r="Z53" s="106"/>
-      <c r="AA53" s="106"/>
-      <c r="AB53" s="106"/>
+      <c r="S53" s="105"/>
+      <c r="T53" s="105"/>
+      <c r="U53" s="105"/>
+      <c r="V53" s="105"/>
+      <c r="W53" s="105"/>
+      <c r="X53" s="105"/>
+      <c r="Y53" s="105"/>
+      <c r="Z53" s="105"/>
+      <c r="AA53" s="105"/>
+      <c r="AB53" s="105"/>
       <c r="AC53" s="27"/>
       <c r="AH53" s="22"/>
       <c r="AI53" s="22"/>
@@ -3715,22 +3715,22 @@
       <c r="AC54" s="27"/>
     </row>
     <row r="55" spans="2:43">
-      <c r="B55" s="101" t="s">
+      <c r="B55" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="101"/>
-      <c r="D55" s="101"/>
-      <c r="E55" s="101"/>
-      <c r="F55" s="101"/>
-      <c r="G55" s="101"/>
-      <c r="H55" s="101"/>
-      <c r="I55" s="101"/>
-      <c r="J55" s="101"/>
-      <c r="K55" s="101"/>
-      <c r="L55" s="101"/>
-      <c r="M55" s="101"/>
-      <c r="N55" s="101"/>
-      <c r="O55" s="101"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="106"/>
+      <c r="E55" s="106"/>
+      <c r="F55" s="106"/>
+      <c r="G55" s="106"/>
+      <c r="H55" s="106"/>
+      <c r="I55" s="106"/>
+      <c r="J55" s="106"/>
+      <c r="K55" s="106"/>
+      <c r="L55" s="106"/>
+      <c r="M55" s="106"/>
+      <c r="N55" s="106"/>
+      <c r="O55" s="106"/>
       <c r="R55" s="28"/>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
@@ -3745,272 +3745,272 @@
       <c r="AC55" s="30"/>
     </row>
     <row r="56" spans="2:43">
-      <c r="B56" s="101"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
-      <c r="E56" s="101"/>
-      <c r="F56" s="101"/>
-      <c r="G56" s="101"/>
-      <c r="H56" s="101"/>
-      <c r="I56" s="101"/>
-      <c r="J56" s="101"/>
-      <c r="K56" s="101"/>
-      <c r="L56" s="101"/>
-      <c r="M56" s="101"/>
-      <c r="N56" s="101"/>
-      <c r="O56" s="101"/>
+      <c r="B56" s="106"/>
+      <c r="C56" s="106"/>
+      <c r="D56" s="106"/>
+      <c r="E56" s="106"/>
+      <c r="F56" s="106"/>
+      <c r="G56" s="106"/>
+      <c r="H56" s="106"/>
+      <c r="I56" s="106"/>
+      <c r="J56" s="106"/>
+      <c r="K56" s="106"/>
+      <c r="L56" s="106"/>
+      <c r="M56" s="106"/>
+      <c r="N56" s="106"/>
+      <c r="O56" s="106"/>
     </row>
     <row r="58" spans="2:43" ht="17.25">
-      <c r="B58" s="109" t="s">
+      <c r="B58" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="109"/>
-      <c r="D58" s="109"/>
-      <c r="E58" s="109"/>
-      <c r="F58" s="109"/>
-      <c r="G58" s="109"/>
-      <c r="H58" s="109"/>
-      <c r="I58" s="109"/>
-      <c r="J58" s="109"/>
-      <c r="K58" s="109"/>
-      <c r="L58" s="109"/>
-      <c r="M58" s="109"/>
-      <c r="N58" s="109"/>
-      <c r="O58" s="109"/>
-      <c r="Q58" s="117" t="s">
+      <c r="C58" s="101"/>
+      <c r="D58" s="101"/>
+      <c r="E58" s="101"/>
+      <c r="F58" s="101"/>
+      <c r="G58" s="101"/>
+      <c r="H58" s="101"/>
+      <c r="I58" s="101"/>
+      <c r="J58" s="101"/>
+      <c r="K58" s="101"/>
+      <c r="L58" s="101"/>
+      <c r="M58" s="101"/>
+      <c r="N58" s="101"/>
+      <c r="O58" s="101"/>
+      <c r="Q58" s="102" t="s">
         <v>169</v>
       </c>
-      <c r="R58" s="117"/>
-      <c r="S58" s="117"/>
-      <c r="T58" s="117"/>
-      <c r="U58" s="117"/>
-      <c r="V58" s="117"/>
-      <c r="W58" s="117"/>
-      <c r="X58" s="117"/>
-      <c r="Y58" s="117"/>
-      <c r="Z58" s="117"/>
-      <c r="AA58" s="117"/>
-      <c r="AB58" s="117"/>
-      <c r="AC58" s="117"/>
-      <c r="AD58" s="117"/>
+      <c r="R58" s="102"/>
+      <c r="S58" s="102"/>
+      <c r="T58" s="102"/>
+      <c r="U58" s="102"/>
+      <c r="V58" s="102"/>
+      <c r="W58" s="102"/>
+      <c r="X58" s="102"/>
+      <c r="Y58" s="102"/>
+      <c r="Z58" s="102"/>
+      <c r="AA58" s="102"/>
+      <c r="AB58" s="102"/>
+      <c r="AC58" s="102"/>
+      <c r="AD58" s="102"/>
     </row>
     <row r="60" spans="2:43" ht="17.25">
-      <c r="B60" s="102" t="s">
+      <c r="B60" s="103" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="102"/>
-      <c r="D60" s="102"/>
-      <c r="E60" s="102"/>
-      <c r="F60" s="102"/>
-      <c r="G60" s="102"/>
-      <c r="H60" s="102"/>
-      <c r="I60" s="102"/>
-      <c r="J60" s="102"/>
-      <c r="K60" s="102"/>
-      <c r="L60" s="102"/>
-      <c r="M60" s="102"/>
-      <c r="N60" s="102"/>
-      <c r="O60" s="102"/>
+      <c r="C60" s="103"/>
+      <c r="D60" s="103"/>
+      <c r="E60" s="103"/>
+      <c r="F60" s="103"/>
+      <c r="G60" s="103"/>
+      <c r="H60" s="103"/>
+      <c r="I60" s="103"/>
+      <c r="J60" s="103"/>
+      <c r="K60" s="103"/>
+      <c r="L60" s="103"/>
+      <c r="M60" s="103"/>
+      <c r="N60" s="103"/>
+      <c r="O60" s="103"/>
       <c r="Q60" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="2:43">
-      <c r="B61" s="102"/>
-      <c r="C61" s="102"/>
-      <c r="D61" s="102"/>
-      <c r="E61" s="102"/>
-      <c r="F61" s="102"/>
-      <c r="G61" s="102"/>
-      <c r="H61" s="102"/>
-      <c r="I61" s="102"/>
-      <c r="J61" s="102"/>
-      <c r="K61" s="102"/>
-      <c r="L61" s="102"/>
-      <c r="M61" s="102"/>
-      <c r="N61" s="102"/>
-      <c r="O61" s="102"/>
+      <c r="B61" s="103"/>
+      <c r="C61" s="103"/>
+      <c r="D61" s="103"/>
+      <c r="E61" s="103"/>
+      <c r="F61" s="103"/>
+      <c r="G61" s="103"/>
+      <c r="H61" s="103"/>
+      <c r="I61" s="103"/>
+      <c r="J61" s="103"/>
+      <c r="K61" s="103"/>
+      <c r="L61" s="103"/>
+      <c r="M61" s="103"/>
+      <c r="N61" s="103"/>
+      <c r="O61" s="103"/>
     </row>
     <row r="62" spans="2:43">
-      <c r="Q62" s="101" t="s">
+      <c r="Q62" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="R62" s="101"/>
-      <c r="S62" s="101"/>
-      <c r="T62" s="101"/>
-      <c r="U62" s="101"/>
-      <c r="V62" s="101"/>
-      <c r="W62" s="101"/>
-      <c r="X62" s="101"/>
-      <c r="Y62" s="101"/>
-      <c r="Z62" s="101"/>
-      <c r="AA62" s="101"/>
-      <c r="AB62" s="101"/>
-      <c r="AC62" s="101"/>
-      <c r="AD62" s="101"/>
+      <c r="R62" s="106"/>
+      <c r="S62" s="106"/>
+      <c r="T62" s="106"/>
+      <c r="U62" s="106"/>
+      <c r="V62" s="106"/>
+      <c r="W62" s="106"/>
+      <c r="X62" s="106"/>
+      <c r="Y62" s="106"/>
+      <c r="Z62" s="106"/>
+      <c r="AA62" s="106"/>
+      <c r="AB62" s="106"/>
+      <c r="AC62" s="106"/>
+      <c r="AD62" s="106"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1">
-      <c r="B63" s="102" t="s">
+      <c r="B63" s="103" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="102"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="102"/>
-      <c r="F63" s="102"/>
-      <c r="G63" s="102"/>
-      <c r="H63" s="102"/>
-      <c r="I63" s="102"/>
-      <c r="J63" s="102"/>
-      <c r="K63" s="102"/>
-      <c r="L63" s="102"/>
-      <c r="M63" s="102"/>
-      <c r="N63" s="102"/>
-      <c r="O63" s="102"/>
-      <c r="Q63" s="101"/>
-      <c r="R63" s="101"/>
-      <c r="S63" s="101"/>
-      <c r="T63" s="101"/>
-      <c r="U63" s="101"/>
-      <c r="V63" s="101"/>
-      <c r="W63" s="101"/>
-      <c r="X63" s="101"/>
-      <c r="Y63" s="101"/>
-      <c r="Z63" s="101"/>
-      <c r="AA63" s="101"/>
-      <c r="AB63" s="101"/>
-      <c r="AC63" s="101"/>
-      <c r="AD63" s="101"/>
+      <c r="C63" s="103"/>
+      <c r="D63" s="103"/>
+      <c r="E63" s="103"/>
+      <c r="F63" s="103"/>
+      <c r="G63" s="103"/>
+      <c r="H63" s="103"/>
+      <c r="I63" s="103"/>
+      <c r="J63" s="103"/>
+      <c r="K63" s="103"/>
+      <c r="L63" s="103"/>
+      <c r="M63" s="103"/>
+      <c r="N63" s="103"/>
+      <c r="O63" s="103"/>
+      <c r="Q63" s="106"/>
+      <c r="R63" s="106"/>
+      <c r="S63" s="106"/>
+      <c r="T63" s="106"/>
+      <c r="U63" s="106"/>
+      <c r="V63" s="106"/>
+      <c r="W63" s="106"/>
+      <c r="X63" s="106"/>
+      <c r="Y63" s="106"/>
+      <c r="Z63" s="106"/>
+      <c r="AA63" s="106"/>
+      <c r="AB63" s="106"/>
+      <c r="AC63" s="106"/>
+      <c r="AD63" s="106"/>
     </row>
     <row r="64" spans="2:43">
-      <c r="B64" s="102"/>
-      <c r="C64" s="102"/>
-      <c r="D64" s="102"/>
-      <c r="E64" s="102"/>
-      <c r="F64" s="102"/>
-      <c r="G64" s="102"/>
-      <c r="H64" s="102"/>
-      <c r="I64" s="102"/>
-      <c r="J64" s="102"/>
-      <c r="K64" s="102"/>
-      <c r="L64" s="102"/>
-      <c r="M64" s="102"/>
-      <c r="N64" s="102"/>
-      <c r="O64" s="102"/>
+      <c r="B64" s="103"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="103"/>
+      <c r="E64" s="103"/>
+      <c r="F64" s="103"/>
+      <c r="G64" s="103"/>
+      <c r="H64" s="103"/>
+      <c r="I64" s="103"/>
+      <c r="J64" s="103"/>
+      <c r="K64" s="103"/>
+      <c r="L64" s="103"/>
+      <c r="M64" s="103"/>
+      <c r="N64" s="103"/>
+      <c r="O64" s="103"/>
     </row>
     <row r="65" spans="2:30" ht="17.25">
-      <c r="B65" s="102"/>
-      <c r="C65" s="102"/>
-      <c r="D65" s="102"/>
-      <c r="E65" s="102"/>
-      <c r="F65" s="102"/>
-      <c r="G65" s="102"/>
-      <c r="H65" s="102"/>
-      <c r="I65" s="102"/>
-      <c r="J65" s="102"/>
-      <c r="K65" s="102"/>
-      <c r="L65" s="102"/>
-      <c r="M65" s="102"/>
-      <c r="N65" s="102"/>
-      <c r="O65" s="102"/>
+      <c r="B65" s="103"/>
+      <c r="C65" s="103"/>
+      <c r="D65" s="103"/>
+      <c r="E65" s="103"/>
+      <c r="F65" s="103"/>
+      <c r="G65" s="103"/>
+      <c r="H65" s="103"/>
+      <c r="I65" s="103"/>
+      <c r="J65" s="103"/>
+      <c r="K65" s="103"/>
+      <c r="L65" s="103"/>
+      <c r="M65" s="103"/>
+      <c r="N65" s="103"/>
+      <c r="O65" s="103"/>
       <c r="Q65" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="66" spans="2:30">
-      <c r="B66" s="102"/>
-      <c r="C66" s="102"/>
-      <c r="D66" s="102"/>
-      <c r="E66" s="102"/>
-      <c r="F66" s="102"/>
-      <c r="G66" s="102"/>
-      <c r="H66" s="102"/>
-      <c r="I66" s="102"/>
-      <c r="J66" s="102"/>
-      <c r="K66" s="102"/>
-      <c r="L66" s="102"/>
-      <c r="M66" s="102"/>
-      <c r="N66" s="102"/>
-      <c r="O66" s="102"/>
+      <c r="B66" s="103"/>
+      <c r="C66" s="103"/>
+      <c r="D66" s="103"/>
+      <c r="E66" s="103"/>
+      <c r="F66" s="103"/>
+      <c r="G66" s="103"/>
+      <c r="H66" s="103"/>
+      <c r="I66" s="103"/>
+      <c r="J66" s="103"/>
+      <c r="K66" s="103"/>
+      <c r="L66" s="103"/>
+      <c r="M66" s="103"/>
+      <c r="N66" s="103"/>
+      <c r="O66" s="103"/>
     </row>
     <row r="67" spans="2:30" ht="15" customHeight="1">
-      <c r="B67" s="101" t="s">
+      <c r="B67" s="106" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="101"/>
-      <c r="D67" s="101"/>
-      <c r="E67" s="101"/>
-      <c r="F67" s="101"/>
-      <c r="G67" s="101"/>
-      <c r="H67" s="101"/>
-      <c r="I67" s="101"/>
-      <c r="J67" s="101"/>
-      <c r="K67" s="101"/>
-      <c r="L67" s="101"/>
-      <c r="M67" s="101"/>
-      <c r="N67" s="101"/>
-      <c r="O67" s="101"/>
-      <c r="Q67" s="101" t="s">
+      <c r="C67" s="106"/>
+      <c r="D67" s="106"/>
+      <c r="E67" s="106"/>
+      <c r="F67" s="106"/>
+      <c r="G67" s="106"/>
+      <c r="H67" s="106"/>
+      <c r="I67" s="106"/>
+      <c r="J67" s="106"/>
+      <c r="K67" s="106"/>
+      <c r="L67" s="106"/>
+      <c r="M67" s="106"/>
+      <c r="N67" s="106"/>
+      <c r="O67" s="106"/>
+      <c r="Q67" s="106" t="s">
         <v>209</v>
       </c>
-      <c r="R67" s="101"/>
-      <c r="S67" s="101"/>
-      <c r="T67" s="101"/>
-      <c r="U67" s="101"/>
-      <c r="V67" s="101"/>
-      <c r="W67" s="101"/>
-      <c r="X67" s="101"/>
-      <c r="Y67" s="101"/>
-      <c r="Z67" s="101"/>
-      <c r="AA67" s="101"/>
-      <c r="AB67" s="101"/>
-      <c r="AC67" s="101"/>
-      <c r="AD67" s="101"/>
+      <c r="R67" s="106"/>
+      <c r="S67" s="106"/>
+      <c r="T67" s="106"/>
+      <c r="U67" s="106"/>
+      <c r="V67" s="106"/>
+      <c r="W67" s="106"/>
+      <c r="X67" s="106"/>
+      <c r="Y67" s="106"/>
+      <c r="Z67" s="106"/>
+      <c r="AA67" s="106"/>
+      <c r="AB67" s="106"/>
+      <c r="AC67" s="106"/>
+      <c r="AD67" s="106"/>
     </row>
     <row r="68" spans="2:30">
-      <c r="B68" s="101"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="101"/>
-      <c r="F68" s="101"/>
-      <c r="G68" s="101"/>
-      <c r="H68" s="101"/>
-      <c r="I68" s="101"/>
-      <c r="J68" s="101"/>
-      <c r="K68" s="101"/>
-      <c r="L68" s="101"/>
-      <c r="M68" s="101"/>
-      <c r="N68" s="101"/>
-      <c r="O68" s="101"/>
-      <c r="Q68" s="101"/>
-      <c r="R68" s="101"/>
-      <c r="S68" s="101"/>
-      <c r="T68" s="101"/>
-      <c r="U68" s="101"/>
-      <c r="V68" s="101"/>
-      <c r="W68" s="101"/>
-      <c r="X68" s="101"/>
-      <c r="Y68" s="101"/>
-      <c r="Z68" s="101"/>
-      <c r="AA68" s="101"/>
-      <c r="AB68" s="101"/>
-      <c r="AC68" s="101"/>
-      <c r="AD68" s="101"/>
+      <c r="B68" s="106"/>
+      <c r="C68" s="106"/>
+      <c r="D68" s="106"/>
+      <c r="E68" s="106"/>
+      <c r="F68" s="106"/>
+      <c r="G68" s="106"/>
+      <c r="H68" s="106"/>
+      <c r="I68" s="106"/>
+      <c r="J68" s="106"/>
+      <c r="K68" s="106"/>
+      <c r="L68" s="106"/>
+      <c r="M68" s="106"/>
+      <c r="N68" s="106"/>
+      <c r="O68" s="106"/>
+      <c r="Q68" s="106"/>
+      <c r="R68" s="106"/>
+      <c r="S68" s="106"/>
+      <c r="T68" s="106"/>
+      <c r="U68" s="106"/>
+      <c r="V68" s="106"/>
+      <c r="W68" s="106"/>
+      <c r="X68" s="106"/>
+      <c r="Y68" s="106"/>
+      <c r="Z68" s="106"/>
+      <c r="AA68" s="106"/>
+      <c r="AB68" s="106"/>
+      <c r="AC68" s="106"/>
+      <c r="AD68" s="106"/>
     </row>
     <row r="69" spans="2:30">
-      <c r="Q69" s="101"/>
-      <c r="R69" s="101"/>
-      <c r="S69" s="101"/>
-      <c r="T69" s="101"/>
-      <c r="U69" s="101"/>
-      <c r="V69" s="101"/>
-      <c r="W69" s="101"/>
-      <c r="X69" s="101"/>
-      <c r="Y69" s="101"/>
-      <c r="Z69" s="101"/>
-      <c r="AA69" s="101"/>
-      <c r="AB69" s="101"/>
-      <c r="AC69" s="101"/>
-      <c r="AD69" s="101"/>
+      <c r="Q69" s="106"/>
+      <c r="R69" s="106"/>
+      <c r="S69" s="106"/>
+      <c r="T69" s="106"/>
+      <c r="U69" s="106"/>
+      <c r="V69" s="106"/>
+      <c r="W69" s="106"/>
+      <c r="X69" s="106"/>
+      <c r="Y69" s="106"/>
+      <c r="Z69" s="106"/>
+      <c r="AA69" s="106"/>
+      <c r="AB69" s="106"/>
+      <c r="AC69" s="106"/>
+      <c r="AD69" s="106"/>
     </row>
     <row r="70" spans="2:30" ht="17.25">
       <c r="B70" s="10" t="s">
@@ -4023,207 +4023,196 @@
       </c>
     </row>
     <row r="73" spans="2:30">
-      <c r="Q73" s="102" t="s">
+      <c r="Q73" s="103" t="s">
         <v>203</v>
       </c>
-      <c r="R73" s="102"/>
-      <c r="S73" s="102"/>
-      <c r="T73" s="102"/>
-      <c r="U73" s="102"/>
-      <c r="V73" s="102"/>
-      <c r="W73" s="102"/>
-      <c r="X73" s="102"/>
-      <c r="Y73" s="102"/>
-      <c r="Z73" s="102"/>
-      <c r="AA73" s="102"/>
-      <c r="AB73" s="102"/>
-      <c r="AC73" s="102"/>
-      <c r="AD73" s="102"/>
+      <c r="R73" s="103"/>
+      <c r="S73" s="103"/>
+      <c r="T73" s="103"/>
+      <c r="U73" s="103"/>
+      <c r="V73" s="103"/>
+      <c r="W73" s="103"/>
+      <c r="X73" s="103"/>
+      <c r="Y73" s="103"/>
+      <c r="Z73" s="103"/>
+      <c r="AA73" s="103"/>
+      <c r="AB73" s="103"/>
+      <c r="AC73" s="103"/>
+      <c r="AD73" s="103"/>
     </row>
     <row r="74" spans="2:30">
-      <c r="Q74" s="102"/>
-      <c r="R74" s="102"/>
-      <c r="S74" s="102"/>
-      <c r="T74" s="102"/>
-      <c r="U74" s="102"/>
-      <c r="V74" s="102"/>
-      <c r="W74" s="102"/>
-      <c r="X74" s="102"/>
-      <c r="Y74" s="102"/>
-      <c r="Z74" s="102"/>
-      <c r="AA74" s="102"/>
-      <c r="AB74" s="102"/>
-      <c r="AC74" s="102"/>
-      <c r="AD74" s="102"/>
+      <c r="Q74" s="103"/>
+      <c r="R74" s="103"/>
+      <c r="S74" s="103"/>
+      <c r="T74" s="103"/>
+      <c r="U74" s="103"/>
+      <c r="V74" s="103"/>
+      <c r="W74" s="103"/>
+      <c r="X74" s="103"/>
+      <c r="Y74" s="103"/>
+      <c r="Z74" s="103"/>
+      <c r="AA74" s="103"/>
+      <c r="AB74" s="103"/>
+      <c r="AC74" s="103"/>
+      <c r="AD74" s="103"/>
     </row>
     <row r="75" spans="2:30" ht="15" customHeight="1">
-      <c r="Q75" s="102"/>
-      <c r="R75" s="102"/>
-      <c r="S75" s="102"/>
-      <c r="T75" s="102"/>
-      <c r="U75" s="102"/>
-      <c r="V75" s="102"/>
-      <c r="W75" s="102"/>
-      <c r="X75" s="102"/>
-      <c r="Y75" s="102"/>
-      <c r="Z75" s="102"/>
-      <c r="AA75" s="102"/>
-      <c r="AB75" s="102"/>
-      <c r="AC75" s="102"/>
-      <c r="AD75" s="102"/>
+      <c r="Q75" s="103"/>
+      <c r="R75" s="103"/>
+      <c r="S75" s="103"/>
+      <c r="T75" s="103"/>
+      <c r="U75" s="103"/>
+      <c r="V75" s="103"/>
+      <c r="W75" s="103"/>
+      <c r="X75" s="103"/>
+      <c r="Y75" s="103"/>
+      <c r="Z75" s="103"/>
+      <c r="AA75" s="103"/>
+      <c r="AB75" s="103"/>
+      <c r="AC75" s="103"/>
+      <c r="AD75" s="103"/>
     </row>
     <row r="76" spans="2:30">
-      <c r="Q76" s="102"/>
-      <c r="R76" s="102"/>
-      <c r="S76" s="102"/>
-      <c r="T76" s="102"/>
-      <c r="U76" s="102"/>
-      <c r="V76" s="102"/>
-      <c r="W76" s="102"/>
-      <c r="X76" s="102"/>
-      <c r="Y76" s="102"/>
-      <c r="Z76" s="102"/>
-      <c r="AA76" s="102"/>
-      <c r="AB76" s="102"/>
-      <c r="AC76" s="102"/>
-      <c r="AD76" s="102"/>
+      <c r="Q76" s="103"/>
+      <c r="R76" s="103"/>
+      <c r="S76" s="103"/>
+      <c r="T76" s="103"/>
+      <c r="U76" s="103"/>
+      <c r="V76" s="103"/>
+      <c r="W76" s="103"/>
+      <c r="X76" s="103"/>
+      <c r="Y76" s="103"/>
+      <c r="Z76" s="103"/>
+      <c r="AA76" s="103"/>
+      <c r="AB76" s="103"/>
+      <c r="AC76" s="103"/>
+      <c r="AD76" s="103"/>
     </row>
     <row r="77" spans="2:30">
-      <c r="Q77" s="102"/>
-      <c r="R77" s="102"/>
-      <c r="S77" s="102"/>
-      <c r="T77" s="102"/>
-      <c r="U77" s="102"/>
-      <c r="V77" s="102"/>
-      <c r="W77" s="102"/>
-      <c r="X77" s="102"/>
-      <c r="Y77" s="102"/>
-      <c r="Z77" s="102"/>
-      <c r="AA77" s="102"/>
-      <c r="AB77" s="102"/>
-      <c r="AC77" s="102"/>
-      <c r="AD77" s="102"/>
+      <c r="Q77" s="103"/>
+      <c r="R77" s="103"/>
+      <c r="S77" s="103"/>
+      <c r="T77" s="103"/>
+      <c r="U77" s="103"/>
+      <c r="V77" s="103"/>
+      <c r="W77" s="103"/>
+      <c r="X77" s="103"/>
+      <c r="Y77" s="103"/>
+      <c r="Z77" s="103"/>
+      <c r="AA77" s="103"/>
+      <c r="AB77" s="103"/>
+      <c r="AC77" s="103"/>
+      <c r="AD77" s="103"/>
     </row>
     <row r="79" spans="2:30" ht="17.25">
-      <c r="B79" s="109" t="s">
+      <c r="B79" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="109"/>
-      <c r="D79" s="109"/>
-      <c r="E79" s="109"/>
-      <c r="F79" s="109"/>
-      <c r="G79" s="109"/>
-      <c r="H79" s="109"/>
-      <c r="I79" s="109"/>
-      <c r="J79" s="109"/>
-      <c r="K79" s="109"/>
-      <c r="L79" s="109"/>
-      <c r="M79" s="109"/>
-      <c r="N79" s="109"/>
-      <c r="O79" s="109"/>
+      <c r="C79" s="101"/>
+      <c r="D79" s="101"/>
+      <c r="E79" s="101"/>
+      <c r="F79" s="101"/>
+      <c r="G79" s="101"/>
+      <c r="H79" s="101"/>
+      <c r="I79" s="101"/>
+      <c r="J79" s="101"/>
+      <c r="K79" s="101"/>
+      <c r="L79" s="101"/>
+      <c r="M79" s="101"/>
+      <c r="N79" s="101"/>
+      <c r="O79" s="101"/>
       <c r="Q79" s="20" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="81" spans="2:30" ht="15" customHeight="1">
-      <c r="B81" s="101" t="s">
+      <c r="B81" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="C81" s="101"/>
-      <c r="D81" s="101"/>
-      <c r="E81" s="101"/>
-      <c r="F81" s="101"/>
-      <c r="G81" s="101"/>
-      <c r="H81" s="101"/>
-      <c r="I81" s="101"/>
-      <c r="J81" s="101"/>
-      <c r="K81" s="101"/>
-      <c r="L81" s="101"/>
-      <c r="M81" s="101"/>
-      <c r="N81" s="101"/>
-      <c r="O81" s="101"/>
-      <c r="Q81" s="102" t="s">
+      <c r="C81" s="106"/>
+      <c r="D81" s="106"/>
+      <c r="E81" s="106"/>
+      <c r="F81" s="106"/>
+      <c r="G81" s="106"/>
+      <c r="H81" s="106"/>
+      <c r="I81" s="106"/>
+      <c r="J81" s="106"/>
+      <c r="K81" s="106"/>
+      <c r="L81" s="106"/>
+      <c r="M81" s="106"/>
+      <c r="N81" s="106"/>
+      <c r="O81" s="106"/>
+      <c r="Q81" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="R81" s="102"/>
-      <c r="S81" s="102"/>
-      <c r="T81" s="102"/>
-      <c r="U81" s="102"/>
-      <c r="V81" s="102"/>
-      <c r="W81" s="102"/>
-      <c r="X81" s="102"/>
-      <c r="Y81" s="102"/>
-      <c r="Z81" s="102"/>
-      <c r="AA81" s="102"/>
-      <c r="AB81" s="102"/>
-      <c r="AC81" s="102"/>
-      <c r="AD81" s="102"/>
+      <c r="R81" s="103"/>
+      <c r="S81" s="103"/>
+      <c r="T81" s="103"/>
+      <c r="U81" s="103"/>
+      <c r="V81" s="103"/>
+      <c r="W81" s="103"/>
+      <c r="X81" s="103"/>
+      <c r="Y81" s="103"/>
+      <c r="Z81" s="103"/>
+      <c r="AA81" s="103"/>
+      <c r="AB81" s="103"/>
+      <c r="AC81" s="103"/>
+      <c r="AD81" s="103"/>
     </row>
     <row r="82" spans="2:30">
-      <c r="B82" s="101"/>
-      <c r="C82" s="101"/>
-      <c r="D82" s="101"/>
-      <c r="E82" s="101"/>
-      <c r="F82" s="101"/>
-      <c r="G82" s="101"/>
-      <c r="H82" s="101"/>
-      <c r="I82" s="101"/>
-      <c r="J82" s="101"/>
-      <c r="K82" s="101"/>
-      <c r="L82" s="101"/>
-      <c r="M82" s="101"/>
-      <c r="N82" s="101"/>
-      <c r="O82" s="101"/>
-      <c r="Q82" s="102"/>
-      <c r="R82" s="102"/>
-      <c r="S82" s="102"/>
-      <c r="T82" s="102"/>
-      <c r="U82" s="102"/>
-      <c r="V82" s="102"/>
-      <c r="W82" s="102"/>
-      <c r="X82" s="102"/>
-      <c r="Y82" s="102"/>
-      <c r="Z82" s="102"/>
-      <c r="AA82" s="102"/>
-      <c r="AB82" s="102"/>
-      <c r="AC82" s="102"/>
-      <c r="AD82" s="102"/>
+      <c r="B82" s="106"/>
+      <c r="C82" s="106"/>
+      <c r="D82" s="106"/>
+      <c r="E82" s="106"/>
+      <c r="F82" s="106"/>
+      <c r="G82" s="106"/>
+      <c r="H82" s="106"/>
+      <c r="I82" s="106"/>
+      <c r="J82" s="106"/>
+      <c r="K82" s="106"/>
+      <c r="L82" s="106"/>
+      <c r="M82" s="106"/>
+      <c r="N82" s="106"/>
+      <c r="O82" s="106"/>
+      <c r="Q82" s="103"/>
+      <c r="R82" s="103"/>
+      <c r="S82" s="103"/>
+      <c r="T82" s="103"/>
+      <c r="U82" s="103"/>
+      <c r="V82" s="103"/>
+      <c r="W82" s="103"/>
+      <c r="X82" s="103"/>
+      <c r="Y82" s="103"/>
+      <c r="Z82" s="103"/>
+      <c r="AA82" s="103"/>
+      <c r="AB82" s="103"/>
+      <c r="AC82" s="103"/>
+      <c r="AD82" s="103"/>
     </row>
     <row r="83" spans="2:30">
-      <c r="Q83" s="102"/>
-      <c r="R83" s="102"/>
-      <c r="S83" s="102"/>
-      <c r="T83" s="102"/>
-      <c r="U83" s="102"/>
-      <c r="V83" s="102"/>
-      <c r="W83" s="102"/>
-      <c r="X83" s="102"/>
-      <c r="Y83" s="102"/>
-      <c r="Z83" s="102"/>
-      <c r="AA83" s="102"/>
-      <c r="AB83" s="102"/>
-      <c r="AC83" s="102"/>
-      <c r="AD83" s="102"/>
+      <c r="Q83" s="103"/>
+      <c r="R83" s="103"/>
+      <c r="S83" s="103"/>
+      <c r="T83" s="103"/>
+      <c r="U83" s="103"/>
+      <c r="V83" s="103"/>
+      <c r="W83" s="103"/>
+      <c r="X83" s="103"/>
+      <c r="Y83" s="103"/>
+      <c r="Z83" s="103"/>
+      <c r="AA83" s="103"/>
+      <c r="AB83" s="103"/>
+      <c r="AC83" s="103"/>
+      <c r="AD83" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B58:O58"/>
-    <mergeCell ref="B79:O79"/>
-    <mergeCell ref="Q58:AD58"/>
-    <mergeCell ref="B60:O61"/>
-    <mergeCell ref="V48:Z48"/>
-    <mergeCell ref="S50:AB50"/>
-    <mergeCell ref="Q67:AD69"/>
-    <mergeCell ref="B50:O51"/>
-    <mergeCell ref="S33:AB34"/>
-    <mergeCell ref="S37:AB38"/>
-    <mergeCell ref="S42:AB42"/>
-    <mergeCell ref="S45:AB46"/>
-    <mergeCell ref="B55:O56"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="B38:O39"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B45:O46"/>
+    <mergeCell ref="B81:O82"/>
+    <mergeCell ref="Q62:AD63"/>
+    <mergeCell ref="B63:O66"/>
+    <mergeCell ref="B67:O68"/>
+    <mergeCell ref="Q73:AD77"/>
+    <mergeCell ref="Q81:AD83"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B4:O5"/>
     <mergeCell ref="B8:O9"/>
@@ -4240,12 +4229,23 @@
     <mergeCell ref="V40:Z40"/>
     <mergeCell ref="S29:AB29"/>
     <mergeCell ref="S26:AB26"/>
-    <mergeCell ref="B81:O82"/>
-    <mergeCell ref="Q62:AD63"/>
-    <mergeCell ref="B63:O66"/>
-    <mergeCell ref="B67:O68"/>
-    <mergeCell ref="Q73:AD77"/>
-    <mergeCell ref="Q81:AD83"/>
+    <mergeCell ref="S33:AB34"/>
+    <mergeCell ref="S37:AB38"/>
+    <mergeCell ref="S42:AB42"/>
+    <mergeCell ref="S45:AB46"/>
+    <mergeCell ref="B55:O56"/>
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="B38:O39"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="B45:O46"/>
+    <mergeCell ref="B58:O58"/>
+    <mergeCell ref="B79:O79"/>
+    <mergeCell ref="Q58:AD58"/>
+    <mergeCell ref="B60:O61"/>
+    <mergeCell ref="V48:Z48"/>
+    <mergeCell ref="S50:AB50"/>
+    <mergeCell ref="Q67:AD69"/>
+    <mergeCell ref="B50:O51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -71726,8 +71726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B821FE-871F-4FF6-AD12-EEE4379083E0}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -71754,7 +71754,7 @@
         <v>219</v>
       </c>
       <c r="B2" s="100">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1">

</xml_diff>